<commit_message>
Bug Fix for February having < 30 Days
</commit_message>
<xml_diff>
--- a/DriveSummary.xlsx
+++ b/DriveSummary.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2fd3bccd6dbaea2b/GitGud/DriveAssistant/ExcelDriveSummary/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2fd3bccd6dbaea2b/GitGud/ExcelDriveSummary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="78" documentId="13_ncr:1_{3A17151E-37E9-4B2A-B0B5-F67B46E403E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FF5F021D-BC34-4EEE-9612-E8101041C925}"/>
+  <xr:revisionPtr revIDLastSave="260" documentId="13_ncr:1_{3A17151E-37E9-4B2A-B0B5-F67B46E403E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{40217B5C-CB26-4016-873E-45F7A7B07564}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{B12B6E18-E294-4985-A977-422328ADD677}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{B12B6E18-E294-4985-A977-422328ADD677}"/>
   </bookViews>
   <sheets>
-    <sheet name="Stefan" sheetId="9" r:id="rId1"/>
-    <sheet name="Christiaan" sheetId="10" r:id="rId2"/>
-    <sheet name="Derrick" sheetId="11" r:id="rId3"/>
+    <sheet name="Stefan" sheetId="12" r:id="rId1"/>
+    <sheet name="Christiaan" sheetId="13" r:id="rId2"/>
+    <sheet name="Derrick" sheetId="14" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="Username" localSheetId="1">Christiaan!$M$12</definedName>
     <definedName name="Username" localSheetId="2">Derrick!$M$12</definedName>
-    <definedName name="Username">Stefan!$M$12</definedName>
+    <definedName name="Username" localSheetId="0">Stefan!$M$12</definedName>
+    <definedName name="Username">#REF!</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="43">
   <si>
     <t>Driving Profile</t>
   </si>
@@ -165,7 +166,13 @@
     <t>Night Extr or Calc</t>
   </si>
   <si>
-    <t>The predicted status gives a more realistic prediction of the driving status. If the prediction is disable, best case scenario is assumed, which is 50 point drive days and the distance remains in the same bracket.</t>
+    <t>The predicted status gives a more realistic prediction of the driving status. If the rediction is disable, best case scenario is assumed, which is 50 point drive days and the distance remains in the same bracket.</t>
+  </si>
+  <si>
+    <t>Days Past</t>
+  </si>
+  <si>
+    <t>Days Left</t>
   </si>
 </sst>
 </file>
@@ -328,7 +335,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -431,22 +438,25 @@
     <xf numFmtId="1" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -809,15 +819,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D6DB9C08-8008-4685-88EF-7625B0BF4470}" name="NightTimeDrive5" displayName="NightTimeDrive5" ref="I6:J7" headerRowDxfId="20" dataDxfId="18" headerRowBorderDxfId="19">
-  <autoFilter ref="I6:J7" xr:uid="{76285C9C-3E4D-42C9-A22A-CEC4B871EA2B}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{9B737206-4861-491C-AFF8-0806B9FBD2B9}" name="NightTimeDrive55" displayName="NightTimeDrive55" ref="I6:J8" headerRowDxfId="20" dataDxfId="18" headerRowBorderDxfId="19">
+  <autoFilter ref="I6:J8" xr:uid="{76285C9C-3E4D-42C9-A22A-CEC4B871EA2B}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{C0E72B15-22F0-4A1E-9BF1-485BAA0289FD}" name="Time" totalsRowLabel="Total" dataDxfId="17" totalsRowDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{266DE4CB-F75B-4FC2-A9AD-F19C793B859E}" name="Points" totalsRowFunction="sum" dataDxfId="15" totalsRowDxfId="14">
-      <calculatedColumnFormula>2*NightTimeDrive5[[#This Row],[Time]]</calculatedColumnFormula>
+    <tableColumn id="1" xr3:uid="{4CDFE2FA-03D0-42E2-B413-54ABDA820257}" name="Time" totalsRowLabel="Total" dataDxfId="17" totalsRowDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{B4617D46-747E-46F7-A55C-2D798F44322B}" name="Points" totalsRowFunction="sum" dataDxfId="15" totalsRowDxfId="14">
+      <calculatedColumnFormula>2*NightTimeDrive55[[#This Row],[Time]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
@@ -825,15 +835,15 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8D670F5E-57E0-4CF5-9F21-14A26AB990F6}" name="NightTimeDrive53" displayName="NightTimeDrive53" ref="I6:J7" headerRowDxfId="13" dataDxfId="11" headerRowBorderDxfId="12">
-  <autoFilter ref="I6:J7" xr:uid="{76285C9C-3E4D-42C9-A22A-CEC4B871EA2B}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{3792EC66-E1B9-478D-94FA-4C3108FEAE99}" name="NightTimeDrive556" displayName="NightTimeDrive556" ref="I6:J8" headerRowDxfId="13" dataDxfId="11" headerRowBorderDxfId="12">
+  <autoFilter ref="I6:J8" xr:uid="{76285C9C-3E4D-42C9-A22A-CEC4B871EA2B}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{357125C7-5E35-4089-8E6C-3EEB3D594D75}" name="Time" totalsRowLabel="Total" dataDxfId="10" totalsRowDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{604B3A25-ECBA-4308-975C-A6602CA98BC3}" name="Points" totalsRowFunction="sum" dataDxfId="8" totalsRowDxfId="7">
-      <calculatedColumnFormula>2*NightTimeDrive53[[#This Row],[Time]]</calculatedColumnFormula>
+    <tableColumn id="1" xr3:uid="{88910778-1637-4D2B-80E2-415C8D40C1A7}" name="Time" totalsRowLabel="Total" dataDxfId="10" totalsRowDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{44440C7A-8D3D-4506-A003-F6BD2ED6494A}" name="Points" totalsRowFunction="sum" dataDxfId="8" totalsRowDxfId="7">
+      <calculatedColumnFormula>2*NightTimeDrive556[[#This Row],[Time]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
@@ -841,15 +851,15 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{475CE5B6-F486-4F86-B3E8-88E762A9259A}" name="NightTimeDrive534" displayName="NightTimeDrive534" ref="I6:J7" headerRowDxfId="6" dataDxfId="4" headerRowBorderDxfId="5">
-  <autoFilter ref="I6:J7" xr:uid="{76285C9C-3E4D-42C9-A22A-CEC4B871EA2B}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{AC23CF0E-EECE-468C-895A-A6A4DD0C8A7F}" name="NightTimeDrive5567" displayName="NightTimeDrive5567" ref="I6:J8" headerRowDxfId="6" dataDxfId="4" headerRowBorderDxfId="5">
+  <autoFilter ref="I6:J8" xr:uid="{76285C9C-3E4D-42C9-A22A-CEC4B871EA2B}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{AECE4228-B60B-4D36-B77D-ED32905AD113}" name="Time" totalsRowLabel="Total" dataDxfId="3" totalsRowDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{E702B27D-DCEE-42D5-94E6-E3347322CDD3}" name="Points" totalsRowFunction="sum" dataDxfId="1" totalsRowDxfId="0">
-      <calculatedColumnFormula>2*NightTimeDrive534[[#This Row],[Time]]</calculatedColumnFormula>
+    <tableColumn id="1" xr3:uid="{FB075366-4CD4-465B-8DF4-AF4AF6B716C6}" name="Time" totalsRowLabel="Total" dataDxfId="3" totalsRowDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{419A2398-118E-4416-9C11-779DB23DD654}" name="Points" totalsRowFunction="sum" dataDxfId="1" totalsRowDxfId="0">
+      <calculatedColumnFormula>2*NightTimeDrive5567[[#This Row],[Time]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
@@ -1152,15 +1162,13 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D23699A-5EFD-4DFA-954C-AE71C0EC78B1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2FABB0D-788A-4DD4-A917-2A765F4254DC}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="B2:AB50"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1179,36 +1187,38 @@
     <col min="15" max="17" width="9.42578125" style="6" customWidth="1"/>
     <col min="18" max="18" width="2.7109375" style="6" customWidth="1"/>
     <col min="19" max="19" width="9.42578125" style="12" customWidth="1"/>
-    <col min="20" max="22" width="9.42578125" style="6" customWidth="1"/>
+    <col min="20" max="20" width="6.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9" style="6" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="6.85546875" style="6" bestFit="1" customWidth="1"/>
     <col min="23" max="24" width="8.85546875" style="6"/>
     <col min="25" max="25" width="8.85546875" style="6" customWidth="1"/>
     <col min="26" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:28" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="39" t="str">
+      <c r="B2" s="41" t="str">
         <f ca="1">_xlfn.CONCAT("Drive Summary ", M12, " ",TEXT(TODAY(), "mmmm yyyy"))</f>
-        <v>Drive Summary Stefan January 2025</v>
-      </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
+        <v>Drive Summary Stefan February 2025</v>
+      </c>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="41"/>
+      <c r="J2" s="41"/>
     </row>
     <row r="3" spans="2:28" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
-      <c r="J3" s="39"/>
+      <c r="B3" s="41"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="41"/>
+      <c r="I3" s="41"/>
+      <c r="J3" s="41"/>
     </row>
     <row r="5" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
@@ -1216,12 +1226,12 @@
       </c>
       <c r="C5" s="17">
         <f ca="1">MIN(1500, IF($C$16,G7,G6+G13))</f>
-        <v>1492</v>
+        <v>1444.75</v>
       </c>
       <c r="D5"/>
       <c r="E5" s="7" t="str">
         <f ca="1">TEXT(TODAY(), "mmmm yyyy")</f>
-        <v>January 2025</v>
+        <v>February 2025</v>
       </c>
       <c r="F5" s="7" t="s">
         <v>1</v>
@@ -1232,24 +1242,24 @@
       <c r="I5" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="J5" s="37"/>
+      <c r="J5" s="38"/>
       <c r="L5" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="M5" s="37"/>
+      <c r="M5" s="38"/>
       <c r="O5" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="P5" s="40"/>
-      <c r="Q5" s="37"/>
+      <c r="P5" s="37"/>
+      <c r="Q5" s="38"/>
       <c r="S5" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="T5" s="40"/>
-      <c r="U5" s="40"/>
-      <c r="V5" s="37"/>
-      <c r="AA5" s="35"/>
-      <c r="AB5" s="35"/>
+      <c r="T5" s="37"/>
+      <c r="U5" s="37"/>
+      <c r="V5" s="38"/>
+      <c r="AA5" s="39"/>
+      <c r="AB5" s="39"/>
     </row>
     <row r="6" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
@@ -1262,10 +1272,10 @@
         <v>6</v>
       </c>
       <c r="F6" s="22">
-        <v>659</v>
+        <v>902</v>
       </c>
       <c r="G6" s="15">
-        <v>1092</v>
+        <v>1149</v>
       </c>
       <c r="I6" s="7" t="s">
         <v>32</v>
@@ -1310,26 +1320,26 @@
       </c>
       <c r="C7" s="30">
         <f>IF( AND( M8&lt;=M14+M15, M8&gt;=M14-M15 ), M8, M14)</f>
-        <v>300</v>
+        <v>240</v>
       </c>
       <c r="D7" s="9"/>
       <c r="E7" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F7" s="17">
-        <f ca="1">F6/(DAY(TODAY())-1)*DAY(EOMONTH(TODAY(), 0))</f>
-        <v>888.21739130434776</v>
+        <f ca="1">F6/M18*M17</f>
+        <v>1052.3333333333335</v>
       </c>
       <c r="G7" s="17">
-        <f ca="1">G6/(DAY(TODAY())-1)*DAY(EOMONTH(TODAY(), 0))</f>
-        <v>1471.8260869565217</v>
+        <f ca="1">G6/M18*M17</f>
+        <v>1340.5</v>
       </c>
       <c r="I7" s="1">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="J7" s="1">
-        <f>2*NightTimeDrive5[[#This Row],[Time]]</f>
-        <v>0</v>
+        <f>2*NightTimeDrive55[[#This Row],[Time]]</f>
+        <v>46</v>
       </c>
       <c r="L7" s="1" t="s">
         <v>14</v>
@@ -1366,14 +1376,21 @@
       </c>
       <c r="C8" s="32">
         <f>VLOOKUP(IF(C16,F7,F6),O7:Q21,3,TRUE)</f>
-        <v>220</v>
+        <v>180</v>
       </c>
       <c r="F8"/>
+      <c r="I8" s="35">
+        <v>7</v>
+      </c>
+      <c r="J8" s="35">
+        <f>2*NightTimeDrive55[[#This Row],[Time]]</f>
+        <v>14</v>
+      </c>
       <c r="L8" s="33" t="s">
         <v>30</v>
       </c>
       <c r="M8" s="22">
-        <v>282</v>
+        <v>240</v>
       </c>
       <c r="O8" s="1">
         <v>150</v>
@@ -1442,23 +1459,23 @@
       </c>
       <c r="C10" s="8">
         <f ca="1">SUM(C5:C9)</f>
-        <v>2612</v>
+        <v>2464.75</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F10" s="16">
-        <f ca="1">F6/(DAY(TODAY())-1)</f>
-        <v>28.652173913043477</v>
+        <f ca="1">F6/M18</f>
+        <v>37.583333333333336</v>
       </c>
       <c r="G10" s="16">
-        <f ca="1">G6/(DAY(TODAY())-1)</f>
-        <v>47.478260869565219</v>
+        <f ca="1">G6/M18</f>
+        <v>47.875</v>
       </c>
       <c r="L10" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="M10" s="37"/>
+      <c r="M10" s="38"/>
       <c r="O10" s="1">
         <v>450</v>
       </c>
@@ -1518,7 +1535,7 @@
       </c>
       <c r="C12" s="1" t="str">
         <f ca="1">VLOOKUP(C10,S7:U11,3,TRUE)</f>
-        <v>Diamond</v>
+        <v>Gold</v>
       </c>
       <c r="D12" s="9"/>
       <c r="E12" s="18"/>
@@ -1551,25 +1568,25 @@
         <v>23</v>
       </c>
       <c r="C13" s="26">
-        <v>1383.96</v>
+        <v>2276.7800000000002</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F13" s="17">
+      <c r="F13" s="17" t="str">
         <f ca="1">IF(C8-M13&lt;=20, "Unlimited", INT(M13/20)*150 +VLOOKUP(F6,O7:Q21,2,TRUE) -F6)</f>
-        <v>840</v>
-      </c>
-      <c r="G13" s="1">
-        <f ca="1">50*(DAY(EOMONTH(TODAY(), 0))-DAY(TODAY()-1))</f>
-        <v>400</v>
+        <v>Unlimited</v>
+      </c>
+      <c r="G13" s="17">
+        <f ca="1">50*M19 + IF(M17&lt;30,(30-M17)*G10,0)</f>
+        <v>295.75</v>
       </c>
       <c r="L13" s="1" t="s">
         <v>37</v>
       </c>
       <c r="M13" s="1">
         <f ca="1">C10-VLOOKUP(C10,S7:U11,1,TRUE)</f>
-        <v>112</v>
+        <v>264.75</v>
       </c>
       <c r="O13" s="1">
         <v>900</v>
@@ -1590,16 +1607,16 @@
         <v>26</v>
       </c>
       <c r="C14" s="8">
-        <f ca="1">MIN(C13,C10)*VLOOKUP(C12,U6:V11,2,FALSE)*10</f>
-        <v>6919.8</v>
+        <f ca="1">C13*VLOOKUP(C12,U6:V11,2,FALSE)*10</f>
+        <v>7968.7300000000005</v>
       </c>
       <c r="I14" s="9"/>
       <c r="L14" s="33" t="s">
         <v>30</v>
       </c>
       <c r="M14" s="1">
-        <f>300-SUM(NightTimeDrive5[Points])</f>
-        <v>300</v>
+        <f>300-SUM(NightTimeDrive55[Points])</f>
+        <v>240</v>
       </c>
       <c r="O14" s="1">
         <v>1050</v>
@@ -1622,7 +1639,7 @@
         <v>38</v>
       </c>
       <c r="M15" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="O15" s="1">
         <v>1200</v>
@@ -1653,7 +1670,7 @@
       </c>
       <c r="M16" s="1" t="str">
         <f>IF( AND( M8&lt;=M14+M15, M8&gt;=M14-M15 ), "Extract", "Calculate")</f>
-        <v>Calculate</v>
+        <v>Extract</v>
       </c>
       <c r="O16" s="1">
         <v>1350</v>
@@ -1670,17 +1687,25 @@
       <c r="W16"/>
     </row>
     <row r="17" spans="2:27" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="38" t="s">
+      <c r="B17" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="C17" s="38"/>
-      <c r="D17" s="38"/>
-      <c r="E17" s="38"/>
-      <c r="F17" s="38"/>
-      <c r="G17" s="38"/>
-      <c r="H17" s="38"/>
-      <c r="I17" s="38"/>
-      <c r="J17" s="38"/>
+      <c r="C17" s="40"/>
+      <c r="D17" s="40"/>
+      <c r="E17" s="40"/>
+      <c r="F17" s="40"/>
+      <c r="G17" s="40"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
+      <c r="J17" s="40"/>
+      <c r="L17" s="1" t="str">
+        <f ca="1">_xlfn.CONCAT("Days ",TEXT(TODAY(), "mmmm 'yy"))</f>
+        <v>Days February '25</v>
+      </c>
+      <c r="M17" s="1">
+        <f ca="1">DAY(EOMONTH(TODAY(), 0))</f>
+        <v>28</v>
+      </c>
       <c r="O17" s="1">
         <v>1500</v>
       </c>
@@ -1697,15 +1722,22 @@
       <c r="W17"/>
     </row>
     <row r="18" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B18" s="38"/>
-      <c r="C18" s="38"/>
-      <c r="D18" s="38"/>
-      <c r="E18" s="38"/>
-      <c r="F18" s="38"/>
-      <c r="G18" s="38"/>
-      <c r="H18" s="38"/>
-      <c r="I18" s="38"/>
-      <c r="J18" s="38"/>
+      <c r="B18" s="40"/>
+      <c r="C18" s="40"/>
+      <c r="D18" s="40"/>
+      <c r="E18" s="40"/>
+      <c r="F18" s="40"/>
+      <c r="G18" s="40"/>
+      <c r="H18" s="40"/>
+      <c r="I18" s="40"/>
+      <c r="J18" s="40"/>
+      <c r="L18" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="M18" s="1">
+        <f ca="1">DAY(TODAY())-1</f>
+        <v>24</v>
+      </c>
       <c r="O18" s="1">
         <v>1650</v>
       </c>
@@ -1731,6 +1763,13 @@
       <c r="H19" s="24"/>
       <c r="I19" s="24"/>
       <c r="J19" s="24"/>
+      <c r="L19" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M19" s="1">
+        <f ca="1">M17-M18</f>
+        <v>4</v>
+      </c>
       <c r="O19" s="1">
         <v>1800</v>
       </c>
@@ -1944,14 +1983,14 @@
     <protectedRange sqref="F6:G6 C6:C7 C9 C13" name="RequiresInput"/>
   </protectedRanges>
   <mergeCells count="8">
-    <mergeCell ref="AA5:AB5"/>
-    <mergeCell ref="L10:M10"/>
-    <mergeCell ref="B17:J18"/>
     <mergeCell ref="B2:J3"/>
     <mergeCell ref="I5:J5"/>
     <mergeCell ref="L5:M5"/>
     <mergeCell ref="O5:Q5"/>
     <mergeCell ref="S5:V5"/>
+    <mergeCell ref="AA5:AB5"/>
+    <mergeCell ref="L10:M10"/>
+    <mergeCell ref="B17:J18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1962,14 +2001,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1391CDA-85BF-4BE9-B7B2-31A522A6F006}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABD76075-3729-42C6-A69A-398FB6E4AB06}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="B2:AB50"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1989,36 +2028,38 @@
     <col min="15" max="17" width="9.42578125" style="6" hidden="1" customWidth="1"/>
     <col min="18" max="18" width="2.7109375" style="6" hidden="1" customWidth="1"/>
     <col min="19" max="19" width="9.42578125" style="12" hidden="1" customWidth="1"/>
-    <col min="20" max="22" width="9.42578125" style="6" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="6.42578125" style="6" hidden="1" customWidth="1"/>
+    <col min="21" max="21" width="9" style="6" hidden="1" customWidth="1"/>
+    <col min="22" max="22" width="6.85546875" style="6" hidden="1" customWidth="1"/>
     <col min="23" max="24" width="8.85546875" style="6"/>
     <col min="25" max="25" width="8.85546875" style="6" customWidth="1"/>
     <col min="26" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:28" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="39" t="str">
+      <c r="B2" s="41" t="str">
         <f ca="1">_xlfn.CONCAT("Drive Summary ", M12, " ",TEXT(TODAY(), "mmmm yyyy"))</f>
-        <v>Drive Summary Christiaan January 2025</v>
-      </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
+        <v>Drive Summary Christiaan February 2025</v>
+      </c>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="41"/>
+      <c r="J2" s="41"/>
     </row>
     <row r="3" spans="2:28" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
-      <c r="J3" s="39"/>
+      <c r="B3" s="41"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="41"/>
+      <c r="I3" s="41"/>
+      <c r="J3" s="41"/>
     </row>
     <row r="5" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
@@ -2026,12 +2067,12 @@
       </c>
       <c r="C5" s="17">
         <f ca="1">MIN(1500, IF($C$16,G7,G6+G13))</f>
-        <v>1500</v>
+        <v>1480.5</v>
       </c>
       <c r="D5"/>
       <c r="E5" s="7" t="str">
         <f ca="1">TEXT(TODAY(), "mmmm yyyy")</f>
-        <v>January 2025</v>
+        <v>February 2025</v>
       </c>
       <c r="F5" s="7" t="s">
         <v>1</v>
@@ -2042,24 +2083,24 @@
       <c r="I5" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="J5" s="37"/>
+      <c r="J5" s="38"/>
       <c r="L5" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="M5" s="37"/>
+      <c r="M5" s="38"/>
       <c r="O5" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="P5" s="40"/>
-      <c r="Q5" s="37"/>
+      <c r="P5" s="37"/>
+      <c r="Q5" s="38"/>
       <c r="S5" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="T5" s="40"/>
-      <c r="U5" s="40"/>
-      <c r="V5" s="37"/>
-      <c r="AA5" s="35"/>
-      <c r="AB5" s="35"/>
+      <c r="T5" s="37"/>
+      <c r="U5" s="37"/>
+      <c r="V5" s="38"/>
+      <c r="AA5" s="39"/>
+      <c r="AB5" s="39"/>
     </row>
     <row r="6" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
@@ -2072,10 +2113,10 @@
         <v>6</v>
       </c>
       <c r="F6" s="22">
-        <v>1770</v>
+        <v>1746</v>
       </c>
       <c r="G6" s="15">
-        <v>1136</v>
+        <v>1182</v>
       </c>
       <c r="I6" s="7" t="s">
         <v>32</v>
@@ -2120,32 +2161,32 @@
       </c>
       <c r="C7" s="30">
         <f>IF( AND( M8&lt;=M14+M15, M8&gt;=M14-M15 ), M8, M14)</f>
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="D7" s="9"/>
       <c r="E7" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F7" s="17">
-        <f ca="1">F6/(DAY(TODAY())-1)*DAY(EOMONTH(TODAY(), 0))</f>
-        <v>2385.6521739130435</v>
+        <f ca="1">F6/M18*M17</f>
+        <v>2037</v>
       </c>
       <c r="G7" s="17">
-        <f ca="1">G6/(DAY(TODAY())-1)*DAY(EOMONTH(TODAY(), 0))</f>
-        <v>1531.1304347826087</v>
+        <f ca="1">G6/M18*M17</f>
+        <v>1379</v>
       </c>
       <c r="I7" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J7" s="1">
-        <f>2*NightTimeDrive53[[#This Row],[Time]]</f>
-        <v>8</v>
+        <f>2*NightTimeDrive556[[#This Row],[Time]]</f>
+        <v>6</v>
       </c>
       <c r="L7" s="1" t="s">
         <v>14</v>
       </c>
       <c r="M7" s="31">
-        <v>25</v>
+        <v>60</v>
       </c>
       <c r="O7" s="1">
         <v>0</v>
@@ -2179,11 +2220,18 @@
         <v>80</v>
       </c>
       <c r="F8"/>
+      <c r="I8" s="35">
+        <v>0</v>
+      </c>
+      <c r="J8" s="35">
+        <f>2*NightTimeDrive556[[#This Row],[Time]]</f>
+        <v>0</v>
+      </c>
       <c r="L8" s="33" t="s">
         <v>30</v>
       </c>
       <c r="M8" s="22">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="O8" s="1">
         <v>150</v>
@@ -2252,24 +2300,23 @@
       </c>
       <c r="C10" s="8">
         <f ca="1">SUM(C5:C9)</f>
-        <v>2322</v>
+        <v>2304.5</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F10" s="16">
-        <f ca="1">F6/(DAY(TODAY())-1)</f>
-        <v>76.956521739130437</v>
+        <f ca="1">F6/M18</f>
+        <v>72.75</v>
       </c>
       <c r="G10" s="16">
-        <f ca="1">G6/(DAY(TODAY())-1)</f>
-        <v>49.391304347826086</v>
-      </c>
-      <c r="I10" s="9"/>
+        <f ca="1">G6/M18</f>
+        <v>49.25</v>
+      </c>
       <c r="L10" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="M10" s="37"/>
+      <c r="M10" s="38"/>
       <c r="O10" s="1">
         <v>450</v>
       </c>
@@ -2293,6 +2340,7 @@
       </c>
     </row>
     <row r="11" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="I11" s="9"/>
       <c r="L11" s="28" t="s">
         <v>34</v>
       </c>
@@ -2361,7 +2409,7 @@
         <v>23</v>
       </c>
       <c r="C13" s="26">
-        <v>1554.7</v>
+        <v>1879.48</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>24</v>
@@ -2370,17 +2418,16 @@
         <f ca="1">IF(C8-M13&lt;=20, "Unlimited", INT(M13/20)*150 +VLOOKUP(F6,O7:Q21,2,TRUE) -F6)</f>
         <v>Unlimited</v>
       </c>
-      <c r="G13" s="1">
-        <f ca="1">50*(DAY(EOMONTH(TODAY(), 0))-DAY(TODAY()-1))</f>
-        <v>400</v>
-      </c>
-      <c r="I13" s="9"/>
+      <c r="G13" s="17">
+        <f ca="1">50*M19 + IF(M17&lt;30,(30-M17)*G10,0)</f>
+        <v>298.5</v>
+      </c>
       <c r="L13" s="1" t="s">
         <v>37</v>
       </c>
       <c r="M13" s="1">
         <f ca="1">C10-VLOOKUP(C10,S7:U11,1,TRUE)</f>
-        <v>122</v>
+        <v>104.5</v>
       </c>
       <c r="O13" s="1">
         <v>900</v>
@@ -2401,15 +2448,16 @@
         <v>26</v>
       </c>
       <c r="C14" s="8">
-        <f ca="1">MIN(C13,C10)*VLOOKUP(C12,U6:V11,2,FALSE)*10</f>
-        <v>5441.45</v>
-      </c>
+        <f ca="1">C13*VLOOKUP(C12,U6:V11,2,FALSE)*10</f>
+        <v>6578.18</v>
+      </c>
+      <c r="I14" s="9"/>
       <c r="L14" s="33" t="s">
         <v>30</v>
       </c>
       <c r="M14" s="1">
-        <f>300-SUM(NightTimeDrive53[Points])</f>
-        <v>292</v>
+        <f>300-SUM(NightTimeDrive556[Points])</f>
+        <v>294</v>
       </c>
       <c r="O14" s="1">
         <v>1050</v>
@@ -2458,14 +2506,12 @@
       <c r="C16" s="23" t="b">
         <v>0</v>
       </c>
-      <c r="I16" s="24"/>
-      <c r="J16" s="24"/>
       <c r="L16" s="1" t="s">
         <v>39</v>
       </c>
       <c r="M16" s="1" t="str">
         <f>IF( AND( M8&lt;=M14+M15, M8&gt;=M14-M15 ), "Extract", "Calculate")</f>
-        <v>Extract</v>
+        <v>Calculate</v>
       </c>
       <c r="O16" s="1">
         <v>1350</v>
@@ -2482,17 +2528,25 @@
       <c r="W16"/>
     </row>
     <row r="17" spans="2:27" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="38" t="s">
+      <c r="B17" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="C17" s="38"/>
-      <c r="D17" s="38"/>
-      <c r="E17" s="38"/>
-      <c r="F17" s="38"/>
-      <c r="G17" s="38"/>
-      <c r="H17" s="38"/>
-      <c r="I17" s="38"/>
-      <c r="J17" s="38"/>
+      <c r="C17" s="40"/>
+      <c r="D17" s="40"/>
+      <c r="E17" s="40"/>
+      <c r="F17" s="40"/>
+      <c r="G17" s="40"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
+      <c r="J17" s="40"/>
+      <c r="L17" s="1" t="str">
+        <f ca="1">_xlfn.CONCAT("Days ",TEXT(TODAY(), "mmmm 'yy"))</f>
+        <v>Days February '25</v>
+      </c>
+      <c r="M17" s="1">
+        <f ca="1">DAY(EOMONTH(TODAY(), 0))</f>
+        <v>28</v>
+      </c>
       <c r="O17" s="1">
         <v>1500</v>
       </c>
@@ -2509,15 +2563,22 @@
       <c r="W17"/>
     </row>
     <row r="18" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B18" s="38"/>
-      <c r="C18" s="38"/>
-      <c r="D18" s="38"/>
-      <c r="E18" s="38"/>
-      <c r="F18" s="38"/>
-      <c r="G18" s="38"/>
-      <c r="H18" s="38"/>
-      <c r="I18" s="38"/>
-      <c r="J18" s="38"/>
+      <c r="B18" s="40"/>
+      <c r="C18" s="40"/>
+      <c r="D18" s="40"/>
+      <c r="E18" s="40"/>
+      <c r="F18" s="40"/>
+      <c r="G18" s="40"/>
+      <c r="H18" s="40"/>
+      <c r="I18" s="40"/>
+      <c r="J18" s="40"/>
+      <c r="L18" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="M18" s="1">
+        <f ca="1">DAY(TODAY())-1</f>
+        <v>24</v>
+      </c>
       <c r="O18" s="1">
         <v>1650</v>
       </c>
@@ -2541,6 +2602,15 @@
       <c r="F19" s="24"/>
       <c r="G19" s="24"/>
       <c r="H19" s="24"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
+      <c r="L19" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M19" s="1">
+        <f ca="1">M17-M18</f>
+        <v>4</v>
+      </c>
       <c r="O19" s="1">
         <v>1800</v>
       </c>
@@ -2646,8 +2716,6 @@
       <c r="U29" s="2"/>
     </row>
     <row r="30" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="I30" s="13"/>
-      <c r="J30" s="13"/>
       <c r="S30" s="6"/>
       <c r="U30" s="2"/>
     </row>
@@ -2655,6 +2723,8 @@
       <c r="E31" s="18"/>
       <c r="F31" s="18"/>
       <c r="G31" s="19"/>
+      <c r="I31" s="13"/>
+      <c r="J31" s="13"/>
       <c r="S31" s="6"/>
       <c r="U31" s="2"/>
     </row>
@@ -2754,14 +2824,14 @@
     <protectedRange sqref="F6:G6 C6:C7 C9 C13" name="RequiresInput"/>
   </protectedRanges>
   <mergeCells count="8">
-    <mergeCell ref="B17:J18"/>
-    <mergeCell ref="AA5:AB5"/>
-    <mergeCell ref="L10:M10"/>
     <mergeCell ref="B2:J3"/>
     <mergeCell ref="I5:J5"/>
     <mergeCell ref="L5:M5"/>
     <mergeCell ref="O5:Q5"/>
     <mergeCell ref="S5:V5"/>
+    <mergeCell ref="AA5:AB5"/>
+    <mergeCell ref="L10:M10"/>
+    <mergeCell ref="B17:J18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2772,14 +2842,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05A4AB4F-6F90-4885-96BB-E2ED1276FA58}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72BE0023-486A-4D7D-A918-15E74A31FF28}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="B2:AB50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2799,36 +2869,38 @@
     <col min="15" max="17" width="9.42578125" style="6" hidden="1" customWidth="1"/>
     <col min="18" max="18" width="2.7109375" style="6" hidden="1" customWidth="1"/>
     <col min="19" max="19" width="9.42578125" style="12" hidden="1" customWidth="1"/>
-    <col min="20" max="22" width="9.42578125" style="6" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="6.42578125" style="6" hidden="1" customWidth="1"/>
+    <col min="21" max="21" width="9" style="6" hidden="1" customWidth="1"/>
+    <col min="22" max="22" width="6.85546875" style="6" hidden="1" customWidth="1"/>
     <col min="23" max="24" width="8.85546875" style="6"/>
     <col min="25" max="25" width="8.85546875" style="6" customWidth="1"/>
     <col min="26" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:28" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="39" t="str">
+      <c r="B2" s="41" t="str">
         <f ca="1">_xlfn.CONCAT("Drive Summary ", M12, " ",TEXT(TODAY(), "mmmm yyyy"))</f>
-        <v>Drive Summary Derrick January 2025</v>
-      </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
+        <v>Drive Summary Derrick February 2025</v>
+      </c>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="41"/>
+      <c r="J2" s="41"/>
     </row>
     <row r="3" spans="2:28" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
-      <c r="J3" s="39"/>
+      <c r="B3" s="41"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="41"/>
+      <c r="I3" s="41"/>
+      <c r="J3" s="41"/>
     </row>
     <row r="5" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
@@ -2836,12 +2908,12 @@
       </c>
       <c r="C5" s="17">
         <f ca="1">MIN(1500, IF($C$16,G7,G6+G13))</f>
-        <v>1482</v>
+        <v>1468.5833333333333</v>
       </c>
       <c r="D5"/>
       <c r="E5" s="7" t="str">
         <f ca="1">TEXT(TODAY(), "mmmm yyyy")</f>
-        <v>January 2025</v>
+        <v>February 2025</v>
       </c>
       <c r="F5" s="7" t="s">
         <v>1</v>
@@ -2852,24 +2924,24 @@
       <c r="I5" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="J5" s="37"/>
+      <c r="J5" s="38"/>
       <c r="L5" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="M5" s="37"/>
+      <c r="M5" s="38"/>
       <c r="O5" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="P5" s="40"/>
-      <c r="Q5" s="37"/>
+      <c r="P5" s="37"/>
+      <c r="Q5" s="38"/>
       <c r="S5" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="T5" s="40"/>
-      <c r="U5" s="40"/>
-      <c r="V5" s="37"/>
-      <c r="AA5" s="35"/>
-      <c r="AB5" s="35"/>
+      <c r="T5" s="37"/>
+      <c r="U5" s="37"/>
+      <c r="V5" s="38"/>
+      <c r="AA5" s="39"/>
+      <c r="AB5" s="39"/>
     </row>
     <row r="6" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
@@ -2882,10 +2954,10 @@
         <v>6</v>
       </c>
       <c r="F6" s="22">
-        <v>711</v>
+        <v>543</v>
       </c>
       <c r="G6" s="15">
-        <v>1082</v>
+        <v>1171</v>
       </c>
       <c r="I6" s="7" t="s">
         <v>32</v>
@@ -2937,25 +3009,25 @@
         <v>12</v>
       </c>
       <c r="F7" s="17">
-        <f ca="1">F6/(DAY(TODAY())-1)*DAY(EOMONTH(TODAY(), 0))</f>
-        <v>958.304347826087</v>
+        <f ca="1">F6/M18*M17</f>
+        <v>633.5</v>
       </c>
       <c r="G7" s="17">
-        <f ca="1">G6/(DAY(TODAY())-1)*DAY(EOMONTH(TODAY(), 0))</f>
-        <v>1458.3478260869565</v>
+        <f ca="1">G6/M18*M17</f>
+        <v>1366.1666666666665</v>
       </c>
       <c r="I7" s="1">
         <v>0</v>
       </c>
       <c r="J7" s="1">
-        <f>2*NightTimeDrive534[[#This Row],[Time]]</f>
+        <f>2*NightTimeDrive5567[[#This Row],[Time]]</f>
         <v>0</v>
       </c>
       <c r="L7" s="1" t="s">
         <v>14</v>
       </c>
       <c r="M7" s="31">
-        <v>200</v>
+        <v>250</v>
       </c>
       <c r="O7" s="1">
         <v>0</v>
@@ -2986,9 +3058,16 @@
       </c>
       <c r="C8" s="32">
         <f>VLOOKUP(IF(C16,F7,F6),O7:Q21,3,TRUE)</f>
-        <v>220</v>
+        <v>240</v>
       </c>
       <c r="F8"/>
+      <c r="I8" s="35">
+        <v>0</v>
+      </c>
+      <c r="J8" s="1">
+        <f>2*NightTimeDrive5567[[#This Row],[Time]]</f>
+        <v>0</v>
+      </c>
       <c r="L8" s="33" t="s">
         <v>30</v>
       </c>
@@ -3062,23 +3141,23 @@
       </c>
       <c r="C10" s="8">
         <f ca="1">SUM(C5:C9)</f>
-        <v>2452</v>
+        <v>2458.583333333333</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F10" s="16">
-        <f ca="1">F6/(DAY(TODAY())-1)</f>
-        <v>30.913043478260871</v>
+        <f ca="1">F6/M18</f>
+        <v>22.625</v>
       </c>
       <c r="G10" s="16">
-        <f ca="1">G6/(DAY(TODAY())-1)</f>
-        <v>47.043478260869563</v>
+        <f ca="1">G6/M18</f>
+        <v>48.791666666666664</v>
       </c>
       <c r="L10" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="M10" s="37"/>
+      <c r="M10" s="38"/>
       <c r="O10" s="1">
         <v>450</v>
       </c>
@@ -3171,7 +3250,7 @@
         <v>23</v>
       </c>
       <c r="C13" s="26">
-        <v>2160.9499999999998</v>
+        <v>784.35</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>24</v>
@@ -3180,16 +3259,16 @@
         <f ca="1">IF(C8-M13&lt;=20, "Unlimited", INT(M13/20)*150 +VLOOKUP(F6,O7:Q21,2,TRUE) -F6)</f>
         <v>Unlimited</v>
       </c>
-      <c r="G13" s="1">
-        <f ca="1">50*(DAY(EOMONTH(TODAY(), 0))-DAY(TODAY()-1))</f>
-        <v>400</v>
+      <c r="G13" s="17">
+        <f ca="1">50*M19 + IF(M17&lt;30,(30-M17)*G10,0)</f>
+        <v>297.58333333333331</v>
       </c>
       <c r="L13" s="1" t="s">
         <v>37</v>
       </c>
       <c r="M13" s="1">
         <f ca="1">C10-VLOOKUP(C10,S7:U11,1,TRUE)</f>
-        <v>252</v>
+        <v>258.58333333333303</v>
       </c>
       <c r="O13" s="1">
         <v>900</v>
@@ -3210,15 +3289,15 @@
         <v>26</v>
       </c>
       <c r="C14" s="8">
-        <f ca="1">MIN(C13,C10)*VLOOKUP(C12,U6:V11,2,FALSE)*10</f>
-        <v>7563.3249999999989</v>
+        <f ca="1">C13*VLOOKUP(C12,U6:V11,2,FALSE)*10</f>
+        <v>2745.2249999999999</v>
       </c>
       <c r="I14" s="9"/>
       <c r="L14" s="33" t="s">
         <v>30</v>
       </c>
       <c r="M14" s="1">
-        <f>300-SUM(NightTimeDrive534[Points])</f>
+        <f>300-SUM(NightTimeDrive5567[Points])</f>
         <v>300</v>
       </c>
       <c r="O14" s="1">
@@ -3290,17 +3369,25 @@
       <c r="W16"/>
     </row>
     <row r="17" spans="2:27" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="38" t="s">
+      <c r="B17" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="C17" s="38"/>
-      <c r="D17" s="38"/>
-      <c r="E17" s="38"/>
-      <c r="F17" s="38"/>
-      <c r="G17" s="38"/>
-      <c r="H17" s="38"/>
-      <c r="I17" s="38"/>
-      <c r="J17" s="38"/>
+      <c r="C17" s="40"/>
+      <c r="D17" s="40"/>
+      <c r="E17" s="40"/>
+      <c r="F17" s="40"/>
+      <c r="G17" s="40"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
+      <c r="J17" s="40"/>
+      <c r="L17" s="1" t="str">
+        <f ca="1">_xlfn.CONCAT("Days ",TEXT(TODAY(), "mmmm 'yy"))</f>
+        <v>Days February '25</v>
+      </c>
+      <c r="M17" s="1">
+        <f ca="1">DAY(EOMONTH(TODAY(), 0))</f>
+        <v>28</v>
+      </c>
       <c r="O17" s="1">
         <v>1500</v>
       </c>
@@ -3317,15 +3404,22 @@
       <c r="W17"/>
     </row>
     <row r="18" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B18" s="38"/>
-      <c r="C18" s="38"/>
-      <c r="D18" s="38"/>
-      <c r="E18" s="38"/>
-      <c r="F18" s="38"/>
-      <c r="G18" s="38"/>
-      <c r="H18" s="38"/>
-      <c r="I18" s="38"/>
-      <c r="J18" s="38"/>
+      <c r="B18" s="40"/>
+      <c r="C18" s="40"/>
+      <c r="D18" s="40"/>
+      <c r="E18" s="40"/>
+      <c r="F18" s="40"/>
+      <c r="G18" s="40"/>
+      <c r="H18" s="40"/>
+      <c r="I18" s="40"/>
+      <c r="J18" s="40"/>
+      <c r="L18" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="M18" s="1">
+        <f ca="1">DAY(TODAY())-1</f>
+        <v>24</v>
+      </c>
       <c r="O18" s="1">
         <v>1650</v>
       </c>
@@ -3351,6 +3445,13 @@
       <c r="H19" s="24"/>
       <c r="I19" s="24"/>
       <c r="J19" s="24"/>
+      <c r="L19" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M19" s="1">
+        <f ca="1">M17-M18</f>
+        <v>4</v>
+      </c>
       <c r="O19" s="1">
         <v>1800</v>
       </c>
@@ -3564,14 +3665,14 @@
     <protectedRange sqref="F6:G6 C6:C7 C9 C13" name="RequiresInput"/>
   </protectedRanges>
   <mergeCells count="8">
-    <mergeCell ref="AA5:AB5"/>
-    <mergeCell ref="L10:M10"/>
-    <mergeCell ref="B17:J18"/>
     <mergeCell ref="B2:J3"/>
     <mergeCell ref="I5:J5"/>
     <mergeCell ref="L5:M5"/>
+    <mergeCell ref="B17:J18"/>
     <mergeCell ref="O5:Q5"/>
     <mergeCell ref="S5:V5"/>
+    <mergeCell ref="AA5:AB5"/>
+    <mergeCell ref="L10:M10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Last Month Drive Status Improved Extraction.
</commit_message>
<xml_diff>
--- a/DriveSummary.xlsx
+++ b/DriveSummary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2fd3bccd6dbaea2b/GitGud/ExcelDriveSummary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="451" documentId="13_ncr:1_{3A17151E-37E9-4B2A-B0B5-F67B46E403E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6EA2AD92-1C52-4260-8AA9-E514D1C0CF8C}"/>
+  <xr:revisionPtr revIDLastSave="582" documentId="13_ncr:1_{3A17151E-37E9-4B2A-B0B5-F67B46E403E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ACE10CB6-6DB1-483B-AEF2-B3B59C6A0A5D}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{B12B6E18-E294-4985-A977-422328ADD677}"/>
   </bookViews>
@@ -243,8 +243,8 @@
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="[$R-1C09]#,##0.00"/>
-    <numFmt numFmtId="167" formatCode="&quot;R&quot;#,##0"/>
-    <numFmt numFmtId="168" formatCode="[$£-809]#,##0"/>
+    <numFmt numFmtId="166" formatCode="&quot;R&quot;#,##0"/>
+    <numFmt numFmtId="167" formatCode="[$£-809]#,##0"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -530,12 +530,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -548,9 +542,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -585,15 +576,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -619,12 +601,12 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -674,6 +656,24 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="5" fillId="7" borderId="5" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -686,6 +686,216 @@
     <cellStyle name="Silver" xfId="3" xr:uid="{14E707C8-7A31-4C64-82D2-79D4451F1D93}"/>
   </cellStyles>
   <dxfs count="131">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD9B3FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFD966"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDBDBDB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF4B084"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF8EA9DB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD9B3FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFD966"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDBDBDB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF4B084"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF8EA9DB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD9B3FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFD966"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDBDBDB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF4B084"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF8EA9DB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD9B3FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFD966"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDBDBDB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF4B084"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF8EA9DB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD9B3FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFD966"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDBDBDB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF4B084"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF8EA9DB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD9B3FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFD966"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDBDBDB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF4B084"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF8EA9DB"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -864,22 +1074,22 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
+        <left style="thin">
           <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
         </bottom>
       </border>
     </dxf>
     <dxf>
       <border outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
         <bottom style="thin">
           <color rgb="FF000000"/>
         </bottom>
@@ -1054,29 +1264,29 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
+        <left style="thin">
           <color rgb="FF000000"/>
-        </bottom>
-      </border>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <border outline="0">
-        <left style="thin">
+        <bottom style="thin">
           <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <fill>
@@ -1095,28 +1305,6 @@
         </right>
         <top/>
         <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -1263,33 +1451,32 @@
       </border>
     </dxf>
     <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
       <border>
         <top style="medium">
           <color rgb="FF000000"/>
         </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -1309,6 +1496,22 @@
           <color rgb="FF000000"/>
         </vertical>
         <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -1319,6 +1522,13 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <fill>
@@ -1338,76 +1548,6 @@
         <top/>
         <bottom/>
       </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD9B3FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFD966"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDBDBDB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF4B084"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF8EA9DB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD9B3FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFD966"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDBDBDB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF4B084"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF8EA9DB"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -1581,30 +1721,30 @@
     <dxf>
       <border outline="0">
         <top style="thin">
-          <color rgb="FF000000"/>
+          <color indexed="64"/>
         </top>
       </border>
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color rgb="FF000000"/>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
         </bottom>
       </border>
     </dxf>
     <dxf>
       <border outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
+        <bottom style="thin">
+          <color indexed="64"/>
         </bottom>
       </border>
     </dxf>
@@ -1771,35 +1911,35 @@
     <dxf>
       <border outline="0">
         <top style="thin">
-          <color rgb="FF000000"/>
+          <color indexed="64"/>
         </top>
       </border>
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <border outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <fill>
@@ -1818,28 +1958,6 @@
         </right>
         <top/>
         <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -1986,33 +2104,32 @@
       </border>
     </dxf>
     <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
       <border>
         <top style="medium">
-          <color rgb="FF000000"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
+          <color indexed="64"/>
+        </top>
       </border>
     </dxf>
     <dxf>
@@ -2021,27 +2138,50 @@
       </font>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
         </right>
         <top/>
         <bottom/>
         <vertical style="thin">
-          <color rgb="FF000000"/>
+          <color indexed="64"/>
         </vertical>
         <horizontal/>
       </border>
     </dxf>
     <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="none">
-          <fgColor rgb="FF000000"/>
+          <fgColor indexed="64"/>
           <bgColor auto="1"/>
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <fill>
@@ -2061,76 +2201,6 @@
         <top/>
         <bottom/>
       </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD9B3FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFD966"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDBDBDB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF4B084"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF8EA9DB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD9B3FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFD966"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDBDBDB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF4B084"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF8EA9DB"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -2304,30 +2374,30 @@
     <dxf>
       <border outline="0">
         <top style="thin">
-          <color indexed="64"/>
+          <color rgb="FF000000"/>
         </top>
       </border>
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
         </bottom>
       </border>
     </dxf>
     <dxf>
       <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
         </bottom>
       </border>
     </dxf>
@@ -2494,35 +2564,35 @@
     <dxf>
       <border outline="0">
         <top style="thin">
-          <color indexed="64"/>
+          <color rgb="FF000000"/>
         </top>
       </border>
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <fill>
@@ -2541,28 +2611,6 @@
         </right>
         <top/>
         <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -2709,33 +2757,32 @@
       </border>
     </dxf>
     <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
       <border>
         <top style="medium">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
           <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
+        </top>
       </border>
     </dxf>
     <dxf>
@@ -2744,27 +2791,50 @@
       </font>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
         </right>
         <top/>
         <bottom/>
         <vertical style="thin">
-          <color indexed="64"/>
+          <color rgb="FF000000"/>
         </vertical>
         <horizontal/>
       </border>
     </dxf>
     <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="none">
-          <fgColor indexed="64"/>
+          <fgColor rgb="FF000000"/>
           <bgColor auto="1"/>
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <fill>
@@ -2784,76 +2854,6 @@
         <top/>
         <bottom/>
       </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD9B3FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFD966"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDBDBDB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF4B084"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF8EA9DB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD9B3FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFD966"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDBDBDB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF4B084"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF8EA9DB"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -2946,19 +2946,23 @@
 </FeaturePropertyBags>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{52D41F9E-201D-494C-B741-54D3661AF0CB}" name="NightTimeDrive1114" displayName="NightTimeDrive1114" ref="E12:G14" totalsRowCount="1" headerRowDxfId="32" dataDxfId="31" totalsRowDxfId="30" headerRowBorderDxfId="28" tableBorderDxfId="29" totalsRowBorderDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{52D41F9E-201D-494C-B741-54D3661AF0CB}" name="NightTimeDrive1114" displayName="NightTimeDrive1114" ref="E12:G14" totalsRowCount="1" headerRowDxfId="128" dataDxfId="126" totalsRowDxfId="124" headerRowBorderDxfId="127" tableBorderDxfId="125" totalsRowBorderDxfId="123">
   <autoFilter ref="E12:G13" xr:uid="{932FCD99-6FCF-4AE6-A66E-74A568E6D121}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{E9820CD1-120D-416C-8D24-0E189A941AF9}" name="Penalty Weight" totalsRowLabel="Total" dataDxfId="25" totalsRowDxfId="26">
+    <tableColumn id="1" xr3:uid="{E9820CD1-120D-416C-8D24-0E189A941AF9}" name="Penalty Weight" totalsRowLabel="Total" dataDxfId="122" totalsRowDxfId="121">
       <calculatedColumnFormula>2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{770CBEF7-6A21-4F31-A449-460FF496815E}" name="Duration" totalsRowFunction="sum" dataDxfId="23" totalsRowDxfId="24"/>
-    <tableColumn id="3" xr3:uid="{16E6B1A8-A2A6-468A-8C73-0F393F4B41CE}" name="Points" totalsRowFunction="sum" dataDxfId="21" totalsRowDxfId="22">
+    <tableColumn id="2" xr3:uid="{770CBEF7-6A21-4F31-A449-460FF496815E}" name="Duration" totalsRowFunction="sum" dataDxfId="120" totalsRowDxfId="119"/>
+    <tableColumn id="3" xr3:uid="{16E6B1A8-A2A6-468A-8C73-0F393F4B41CE}" name="Points" totalsRowFunction="sum" dataDxfId="118" totalsRowDxfId="117">
       <calculatedColumnFormula>NightTimeDrive1114[[#This Row],[Penalty Weight]]*NightTimeDrive1114[[#This Row],[Duration]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2967,7 +2971,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{1160EBD6-A6E3-4181-915B-B8ABBB18A0C2}" name="Table291215" displayName="Table291215" ref="L6:R13" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19" headerRowBorderDxfId="17" tableBorderDxfId="18" totalsRowBorderDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{1160EBD6-A6E3-4181-915B-B8ABBB18A0C2}" name="Table291215" displayName="Table291215" ref="L6:R13" totalsRowShown="0" headerRowDxfId="116" dataDxfId="114" headerRowBorderDxfId="115" tableBorderDxfId="113" totalsRowBorderDxfId="112">
   <autoFilter ref="L6:R13" xr:uid="{E011F3DC-4D15-4380-B07D-61D2F4291EE8}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -2978,20 +2982,20 @@
     <filterColumn colId="6" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{9F8771AF-CF50-4453-B679-BC454065B222}" name="Lower" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{4C8C475B-44BE-4D66-96D4-24EDC8D2FDE2}" name="Upper" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{C2CF2F37-F8EC-43C5-BB1A-40F3F4293DAC}" name="Blue" dataDxfId="13" dataCellStyle="Blue"/>
-    <tableColumn id="4" xr3:uid="{65448F0C-31EF-4CAE-B825-712186EF8E29}" name="Bronze" dataDxfId="12" dataCellStyle="Bronze"/>
-    <tableColumn id="5" xr3:uid="{50DA8696-F485-43D5-BD1F-433F94EC712E}" name="Silver" dataDxfId="11" dataCellStyle="Silver"/>
-    <tableColumn id="6" xr3:uid="{D9FE27AD-9808-43A6-B9BF-5F1BAF5D78B0}" name="Gold" dataDxfId="10" dataCellStyle="Gold"/>
-    <tableColumn id="7" xr3:uid="{9DC7BCD5-87F7-4BEB-9965-BF447806825D}" name="Diamond" dataDxfId="9" dataCellStyle="Diamond"/>
+    <tableColumn id="1" xr3:uid="{9F8771AF-CF50-4453-B679-BC454065B222}" name="Lower" dataDxfId="111"/>
+    <tableColumn id="2" xr3:uid="{4C8C475B-44BE-4D66-96D4-24EDC8D2FDE2}" name="Upper" dataDxfId="110"/>
+    <tableColumn id="3" xr3:uid="{C2CF2F37-F8EC-43C5-BB1A-40F3F4293DAC}" name="Blue" dataDxfId="109" dataCellStyle="Blue"/>
+    <tableColumn id="4" xr3:uid="{65448F0C-31EF-4CAE-B825-712186EF8E29}" name="Bronze" dataDxfId="108" dataCellStyle="Bronze"/>
+    <tableColumn id="5" xr3:uid="{50DA8696-F485-43D5-BD1F-433F94EC712E}" name="Silver" dataDxfId="107" dataCellStyle="Silver"/>
+    <tableColumn id="6" xr3:uid="{D9FE27AD-9808-43A6-B9BF-5F1BAF5D78B0}" name="Gold" dataDxfId="106" dataCellStyle="Gold"/>
+    <tableColumn id="7" xr3:uid="{9DC7BCD5-87F7-4BEB-9965-BF447806825D}" name="Diamond" dataDxfId="105" dataCellStyle="Diamond"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{773E3023-89B9-4F29-B55D-D429DA394505}" name="Table41316" displayName="Table41316" ref="M26:Q31" totalsRowShown="0" headerRowDxfId="8" headerRowBorderDxfId="6" tableBorderDxfId="7" totalsRowBorderDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{773E3023-89B9-4F29-B55D-D429DA394505}" name="Table41316" displayName="Table41316" ref="M26:Q31" totalsRowShown="0" headerRowDxfId="104" headerRowBorderDxfId="103" tableBorderDxfId="102" totalsRowBorderDxfId="101">
   <autoFilter ref="M26:Q31" xr:uid="{DC26E8D9-5FBB-4486-917F-B1866C4C6343}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -3000,29 +3004,29 @@
     <filterColumn colId="4" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{FED11EC9-AD58-4F5D-A3BF-2F8F6D5282D0}" name="Lower" dataDxfId="4" dataCellStyle="Silver"/>
-    <tableColumn id="2" xr3:uid="{F2569052-4C17-4127-9FBA-B31B3D522A94}" name="Upper" dataDxfId="3" dataCellStyle="Silver"/>
-    <tableColumn id="3" xr3:uid="{65EFAAFB-D8DD-4A4F-AA56-CB3BBDFC28AD}" name="Category" dataDxfId="2" dataCellStyle="Silver"/>
-    <tableColumn id="4" xr3:uid="{2CA1D7B4-D6E7-4D28-98FF-FE0259A7A85B}" name="Fuel %" dataDxfId="1" dataCellStyle="Silver"/>
-    <tableColumn id="5" xr3:uid="{4CB4463C-CAB7-4F04-8814-E6A75BD3E2E6}" name="Color" dataDxfId="0" dataCellStyle="Silver"/>
+    <tableColumn id="1" xr3:uid="{FED11EC9-AD58-4F5D-A3BF-2F8F6D5282D0}" name="Lower" dataDxfId="100" dataCellStyle="Silver"/>
+    <tableColumn id="2" xr3:uid="{F2569052-4C17-4127-9FBA-B31B3D522A94}" name="Upper" dataDxfId="99" dataCellStyle="Silver"/>
+    <tableColumn id="3" xr3:uid="{65EFAAFB-D8DD-4A4F-AA56-CB3BBDFC28AD}" name="Category" dataDxfId="98" dataCellStyle="Silver"/>
+    <tableColumn id="4" xr3:uid="{2CA1D7B4-D6E7-4D28-98FF-FE0259A7A85B}" name="Fuel %" dataDxfId="97" dataCellStyle="Silver"/>
+    <tableColumn id="5" xr3:uid="{4CB4463C-CAB7-4F04-8814-E6A75BD3E2E6}" name="Color" dataDxfId="96" dataCellStyle="Silver"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{2691DD60-8F0D-4A00-BE27-FE334C07FAC0}" name="NightTimeDrive" displayName="NightTimeDrive" ref="E12:G14" totalsRowCount="1" headerRowDxfId="118" dataDxfId="117" totalsRowDxfId="116" headerRowBorderDxfId="114" tableBorderDxfId="115" totalsRowBorderDxfId="113">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{2691DD60-8F0D-4A00-BE27-FE334C07FAC0}" name="NightTimeDrive" displayName="NightTimeDrive" ref="E12:G14" totalsRowCount="1" headerRowDxfId="95" dataDxfId="93" totalsRowDxfId="91" headerRowBorderDxfId="94" tableBorderDxfId="92" totalsRowBorderDxfId="90">
   <autoFilter ref="E12:G13" xr:uid="{932FCD99-6FCF-4AE6-A66E-74A568E6D121}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{DC70D449-17F5-4122-A1BF-3B2E9767E577}" name="Penalty Weight" totalsRowLabel="Total" dataDxfId="111" totalsRowDxfId="112">
+    <tableColumn id="1" xr3:uid="{DC70D449-17F5-4122-A1BF-3B2E9767E577}" name="Penalty Weight" totalsRowLabel="Total" dataDxfId="89" totalsRowDxfId="88">
       <calculatedColumnFormula>2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{C181C36A-8D62-47D8-8D26-3B259CBE4530}" name="Duration" totalsRowFunction="sum" dataDxfId="109" totalsRowDxfId="110"/>
-    <tableColumn id="3" xr3:uid="{904077CA-AF98-4510-BEF4-9B248A3A20F5}" name="Points" totalsRowFunction="sum" dataDxfId="107" totalsRowDxfId="108">
+    <tableColumn id="2" xr3:uid="{C181C36A-8D62-47D8-8D26-3B259CBE4530}" name="Duration" totalsRowFunction="sum" dataDxfId="87" totalsRowDxfId="86"/>
+    <tableColumn id="3" xr3:uid="{904077CA-AF98-4510-BEF4-9B248A3A20F5}" name="Points" totalsRowFunction="sum" dataDxfId="85" totalsRowDxfId="84">
       <calculatedColumnFormula>NightTimeDrive[[#This Row],[Penalty Weight]]*NightTimeDrive[[#This Row],[Duration]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3031,7 +3035,7 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{B05817D9-1883-492B-AB3F-F24E633A8C0A}" name="Table29" displayName="Table29" ref="L6:R13" totalsRowShown="0" headerRowDxfId="106" dataDxfId="105" headerRowBorderDxfId="103" tableBorderDxfId="104" totalsRowBorderDxfId="102">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{B05817D9-1883-492B-AB3F-F24E633A8C0A}" name="Table29" displayName="Table29" ref="L6:R13" totalsRowShown="0" headerRowDxfId="83" dataDxfId="81" headerRowBorderDxfId="82" tableBorderDxfId="80" totalsRowBorderDxfId="79">
   <autoFilter ref="L6:R13" xr:uid="{E011F3DC-4D15-4380-B07D-61D2F4291EE8}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -3042,20 +3046,20 @@
     <filterColumn colId="6" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{1D54ADDF-43E2-4F96-AA0A-08B95EEE5525}" name="Lower" dataDxfId="101"/>
-    <tableColumn id="2" xr3:uid="{8E369D9F-A506-4BE7-9450-D6DF354C5B91}" name="Upper" dataDxfId="100"/>
-    <tableColumn id="3" xr3:uid="{90C9EB12-15B2-4428-96D6-DE91D30E2889}" name="Blue" dataDxfId="99" dataCellStyle="Blue"/>
-    <tableColumn id="4" xr3:uid="{B4A53663-1ECB-453B-B978-91EE1740911A}" name="Bronze" dataDxfId="98" dataCellStyle="Bronze"/>
-    <tableColumn id="5" xr3:uid="{A8DB5A56-B069-4E83-866B-14EF2687BADA}" name="Silver" dataDxfId="97" dataCellStyle="Silver"/>
-    <tableColumn id="6" xr3:uid="{4001DA99-4444-4282-9028-0B13BBB90400}" name="Gold" dataDxfId="96" dataCellStyle="Gold"/>
-    <tableColumn id="7" xr3:uid="{BBFFC5AC-532E-41BE-B430-58B98A15C217}" name="Diamond" dataDxfId="95" dataCellStyle="Diamond"/>
+    <tableColumn id="1" xr3:uid="{1D54ADDF-43E2-4F96-AA0A-08B95EEE5525}" name="Lower" dataDxfId="78"/>
+    <tableColumn id="2" xr3:uid="{8E369D9F-A506-4BE7-9450-D6DF354C5B91}" name="Upper" dataDxfId="77"/>
+    <tableColumn id="3" xr3:uid="{90C9EB12-15B2-4428-96D6-DE91D30E2889}" name="Blue" dataDxfId="76" dataCellStyle="Blue"/>
+    <tableColumn id="4" xr3:uid="{B4A53663-1ECB-453B-B978-91EE1740911A}" name="Bronze" dataDxfId="75" dataCellStyle="Bronze"/>
+    <tableColumn id="5" xr3:uid="{A8DB5A56-B069-4E83-866B-14EF2687BADA}" name="Silver" dataDxfId="74" dataCellStyle="Silver"/>
+    <tableColumn id="6" xr3:uid="{4001DA99-4444-4282-9028-0B13BBB90400}" name="Gold" dataDxfId="73" dataCellStyle="Gold"/>
+    <tableColumn id="7" xr3:uid="{BBFFC5AC-532E-41BE-B430-58B98A15C217}" name="Diamond" dataDxfId="72" dataCellStyle="Diamond"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{42A18A49-3191-4A1B-9245-11E2443B1970}" name="Table4" displayName="Table4" ref="M26:Q31" totalsRowShown="0" headerRowDxfId="94" headerRowBorderDxfId="92" tableBorderDxfId="93" totalsRowBorderDxfId="91">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{42A18A49-3191-4A1B-9245-11E2443B1970}" name="Table4" displayName="Table4" ref="M26:Q31" totalsRowShown="0" headerRowDxfId="71" headerRowBorderDxfId="70" tableBorderDxfId="69" totalsRowBorderDxfId="68">
   <autoFilter ref="M26:Q31" xr:uid="{DC26E8D9-5FBB-4486-917F-B1866C4C6343}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -3064,29 +3068,29 @@
     <filterColumn colId="4" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{59217B13-3B83-4FE5-88CE-31A352DB4072}" name="Lower" dataDxfId="90" dataCellStyle="Silver"/>
-    <tableColumn id="2" xr3:uid="{85A2F208-22D3-439D-9DE4-1ECE40DC05B0}" name="Upper" dataDxfId="89" dataCellStyle="Silver"/>
-    <tableColumn id="3" xr3:uid="{84A9C290-D556-4FE3-92BF-8EA0F1B50652}" name="Category" dataDxfId="88" dataCellStyle="Silver"/>
-    <tableColumn id="4" xr3:uid="{DCE701AB-8DA8-49A4-9822-7012476D8245}" name="Fuel %" dataDxfId="87" dataCellStyle="Silver"/>
-    <tableColumn id="5" xr3:uid="{9C1F6053-54F6-484A-9EAD-AC7FF701777F}" name="Color" dataDxfId="86" dataCellStyle="Silver"/>
+    <tableColumn id="1" xr3:uid="{59217B13-3B83-4FE5-88CE-31A352DB4072}" name="Lower" dataDxfId="67" dataCellStyle="Silver"/>
+    <tableColumn id="2" xr3:uid="{85A2F208-22D3-439D-9DE4-1ECE40DC05B0}" name="Upper" dataDxfId="66" dataCellStyle="Silver"/>
+    <tableColumn id="3" xr3:uid="{84A9C290-D556-4FE3-92BF-8EA0F1B50652}" name="Category" dataDxfId="65" dataCellStyle="Silver"/>
+    <tableColumn id="4" xr3:uid="{DCE701AB-8DA8-49A4-9822-7012476D8245}" name="Fuel %" dataDxfId="64" dataCellStyle="Silver"/>
+    <tableColumn id="5" xr3:uid="{9C1F6053-54F6-484A-9EAD-AC7FF701777F}" name="Color" dataDxfId="63" dataCellStyle="Silver"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{5CE1FAFA-4CDE-4F06-804A-41746F5F5473}" name="NightTimeDrive11" displayName="NightTimeDrive11" ref="E12:G14" totalsRowCount="1" headerRowDxfId="75" dataDxfId="74" totalsRowDxfId="73" headerRowBorderDxfId="71" tableBorderDxfId="72" totalsRowBorderDxfId="70">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{5CE1FAFA-4CDE-4F06-804A-41746F5F5473}" name="NightTimeDrive11" displayName="NightTimeDrive11" ref="E12:G14" totalsRowCount="1" headerRowDxfId="62" dataDxfId="60" totalsRowDxfId="58" headerRowBorderDxfId="61" tableBorderDxfId="59" totalsRowBorderDxfId="57">
   <autoFilter ref="E12:G13" xr:uid="{932FCD99-6FCF-4AE6-A66E-74A568E6D121}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{735D4564-3A90-415B-B47E-5EA90825A97A}" name="Penalty Weight" totalsRowLabel="Total" dataDxfId="68" totalsRowDxfId="69">
+    <tableColumn id="1" xr3:uid="{735D4564-3A90-415B-B47E-5EA90825A97A}" name="Penalty Weight" totalsRowLabel="Total" dataDxfId="56" totalsRowDxfId="55">
       <calculatedColumnFormula>2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{EEF150EB-580C-474F-8688-6A037448742C}" name="Duration" totalsRowFunction="sum" dataDxfId="66" totalsRowDxfId="67"/>
-    <tableColumn id="3" xr3:uid="{5CEA56CD-422B-4282-AD7D-E4F69237A98B}" name="Points" totalsRowFunction="sum" dataDxfId="64" totalsRowDxfId="65">
+    <tableColumn id="2" xr3:uid="{EEF150EB-580C-474F-8688-6A037448742C}" name="Duration" totalsRowFunction="sum" dataDxfId="54" totalsRowDxfId="53"/>
+    <tableColumn id="3" xr3:uid="{5CEA56CD-422B-4282-AD7D-E4F69237A98B}" name="Points" totalsRowFunction="sum" dataDxfId="52" totalsRowDxfId="51">
       <calculatedColumnFormula>NightTimeDrive11[[#This Row],[Penalty Weight]]*NightTimeDrive11[[#This Row],[Duration]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3095,7 +3099,7 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{66027C31-F46F-4630-BA7C-A7D788214406}" name="Table2912" displayName="Table2912" ref="L6:R13" totalsRowShown="0" headerRowDxfId="63" dataDxfId="62" headerRowBorderDxfId="60" tableBorderDxfId="61" totalsRowBorderDxfId="59">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{66027C31-F46F-4630-BA7C-A7D788214406}" name="Table2912" displayName="Table2912" ref="L6:R13" totalsRowShown="0" headerRowDxfId="50" dataDxfId="48" headerRowBorderDxfId="49" tableBorderDxfId="47" totalsRowBorderDxfId="46">
   <autoFilter ref="L6:R13" xr:uid="{E011F3DC-4D15-4380-B07D-61D2F4291EE8}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -3106,20 +3110,20 @@
     <filterColumn colId="6" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{0276F9D3-B063-44DA-ADE6-1070BFDB3D35}" name="Lower" dataDxfId="58"/>
-    <tableColumn id="2" xr3:uid="{A553EDA2-505F-4944-960E-813BAE0280E6}" name="Upper" dataDxfId="57"/>
-    <tableColumn id="3" xr3:uid="{0D70A2B2-3135-468C-A321-4AEC2A2C9C11}" name="Blue" dataDxfId="56" dataCellStyle="Blue"/>
-    <tableColumn id="4" xr3:uid="{E8B32CB2-909D-40E6-8289-BAEBC5F6C299}" name="Bronze" dataDxfId="55" dataCellStyle="Bronze"/>
-    <tableColumn id="5" xr3:uid="{128F56E7-FA96-49D8-BA0E-6D47528F1475}" name="Silver" dataDxfId="54" dataCellStyle="Silver"/>
-    <tableColumn id="6" xr3:uid="{54B51153-77EB-4AD5-A4B1-A65717A58F23}" name="Gold" dataDxfId="53" dataCellStyle="Gold"/>
-    <tableColumn id="7" xr3:uid="{DCB5DC0A-9344-439A-829F-17C180815C46}" name="Diamond" dataDxfId="52" dataCellStyle="Diamond"/>
+    <tableColumn id="1" xr3:uid="{0276F9D3-B063-44DA-ADE6-1070BFDB3D35}" name="Lower" dataDxfId="45"/>
+    <tableColumn id="2" xr3:uid="{A553EDA2-505F-4944-960E-813BAE0280E6}" name="Upper" dataDxfId="44"/>
+    <tableColumn id="3" xr3:uid="{0D70A2B2-3135-468C-A321-4AEC2A2C9C11}" name="Blue" dataDxfId="43" dataCellStyle="Blue"/>
+    <tableColumn id="4" xr3:uid="{E8B32CB2-909D-40E6-8289-BAEBC5F6C299}" name="Bronze" dataDxfId="42" dataCellStyle="Bronze"/>
+    <tableColumn id="5" xr3:uid="{128F56E7-FA96-49D8-BA0E-6D47528F1475}" name="Silver" dataDxfId="41" dataCellStyle="Silver"/>
+    <tableColumn id="6" xr3:uid="{54B51153-77EB-4AD5-A4B1-A65717A58F23}" name="Gold" dataDxfId="40" dataCellStyle="Gold"/>
+    <tableColumn id="7" xr3:uid="{DCB5DC0A-9344-439A-829F-17C180815C46}" name="Diamond" dataDxfId="39" dataCellStyle="Diamond"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{BA3552F5-BA84-40EA-9705-39CDD98F00E4}" name="Table413" displayName="Table413" ref="M26:Q31" totalsRowShown="0" headerRowDxfId="51" headerRowBorderDxfId="49" tableBorderDxfId="50" totalsRowBorderDxfId="48">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{BA3552F5-BA84-40EA-9705-39CDD98F00E4}" name="Table413" displayName="Table413" ref="M26:Q31" totalsRowShown="0" headerRowDxfId="38" headerRowBorderDxfId="37" tableBorderDxfId="36" totalsRowBorderDxfId="35">
   <autoFilter ref="M26:Q31" xr:uid="{DC26E8D9-5FBB-4486-917F-B1866C4C6343}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -3128,11 +3132,11 @@
     <filterColumn colId="4" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{421B8BD1-6ECD-4E7F-B4CC-3E6B400A6616}" name="Lower" dataDxfId="47" dataCellStyle="Silver"/>
-    <tableColumn id="2" xr3:uid="{AC79C6A7-9997-42DA-9554-F726645E1847}" name="Upper" dataDxfId="46" dataCellStyle="Silver"/>
-    <tableColumn id="3" xr3:uid="{86277536-AE35-4170-B2EE-720D4049918D}" name="Category" dataDxfId="45" dataCellStyle="Silver"/>
-    <tableColumn id="4" xr3:uid="{A9D36B79-51B1-4307-9F74-135ECAE6B10E}" name="Fuel %" dataDxfId="44" dataCellStyle="Silver"/>
-    <tableColumn id="5" xr3:uid="{177AEE58-7FAC-4322-86D6-2E43CB79763D}" name="Color" dataDxfId="43" dataCellStyle="Silver"/>
+    <tableColumn id="1" xr3:uid="{421B8BD1-6ECD-4E7F-B4CC-3E6B400A6616}" name="Lower" dataDxfId="34" dataCellStyle="Silver"/>
+    <tableColumn id="2" xr3:uid="{AC79C6A7-9997-42DA-9554-F726645E1847}" name="Upper" dataDxfId="33" dataCellStyle="Silver"/>
+    <tableColumn id="3" xr3:uid="{86277536-AE35-4170-B2EE-720D4049918D}" name="Category" dataDxfId="32" dataCellStyle="Silver"/>
+    <tableColumn id="4" xr3:uid="{A9D36B79-51B1-4307-9F74-135ECAE6B10E}" name="Fuel %" dataDxfId="31" dataCellStyle="Silver"/>
+    <tableColumn id="5" xr3:uid="{177AEE58-7FAC-4322-86D6-2E43CB79763D}" name="Color" dataDxfId="30" dataCellStyle="Silver"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -3441,7 +3445,7 @@
   <dimension ref="B2:AC50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3471,59 +3475,59 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:29" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="24" t="str">
+      <c r="B2" s="65" t="str">
         <f ca="1">_xlfn.CONCAT("Drive Summary ",J18, " ",TEXT(TODAY(), "mmmm yyyy"))</f>
         <v>Drive Summary Stefan March 2025</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="25"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="65"/>
+      <c r="G2" s="65"/>
+      <c r="H2" s="23"/>
     </row>
     <row r="3" spans="2:29" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="25"/>
+      <c r="B3" s="65"/>
+      <c r="C3" s="65"/>
+      <c r="D3" s="65"/>
+      <c r="E3" s="65"/>
+      <c r="F3" s="65"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="23"/>
     </row>
     <row r="5" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B5" s="26" t="s">
+      <c r="B5" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="27" t="s">
+      <c r="C5" s="25" t="s">
         <v>31</v>
       </c>
       <c r="D5"/>
-      <c r="E5" s="26" t="str">
+      <c r="E5" s="24" t="str">
         <f ca="1">TEXT(TODAY(), "mmmm yyyy")</f>
         <v>March 2025</v>
       </c>
-      <c r="F5" s="26" t="s">
+      <c r="F5" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="G5" s="28" t="s">
+      <c r="G5" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="I5" s="29" t="s">
+      <c r="I5" s="64" t="s">
         <v>28</v>
       </c>
-      <c r="J5" s="29"/>
-      <c r="L5" s="29" t="s">
+      <c r="J5" s="64"/>
+      <c r="L5" s="64" t="s">
         <v>11</v>
       </c>
-      <c r="M5" s="29"/>
-      <c r="N5" s="29"/>
-      <c r="O5" s="29"/>
-      <c r="P5" s="29"/>
-      <c r="Q5" s="29"/>
-      <c r="R5" s="29"/>
-      <c r="AB5" s="23"/>
-      <c r="AC5" s="23"/>
+      <c r="M5" s="64"/>
+      <c r="N5" s="64"/>
+      <c r="O5" s="64"/>
+      <c r="P5" s="64"/>
+      <c r="Q5" s="64"/>
+      <c r="R5" s="64"/>
+      <c r="AB5" s="66"/>
+      <c r="AC5" s="66"/>
     </row>
     <row r="6" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
@@ -3536,37 +3540,38 @@
       <c r="E6" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6" s="11">
+        <f>J11</f>
+        <v>700</v>
+      </c>
+      <c r="G6" s="27">
         <v>500</v>
       </c>
-      <c r="G6" s="30">
-        <v>500</v>
-      </c>
-      <c r="I6" s="28" t="s">
+      <c r="I6" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="J6" s="28" t="s">
+      <c r="J6" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="L6" s="28" t="s">
+      <c r="L6" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="M6" s="28" t="s">
+      <c r="M6" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="N6" s="31" t="s">
+      <c r="N6" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="O6" s="32" t="s">
+      <c r="O6" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="P6" s="33" t="s">
+      <c r="P6" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="Q6" s="34" t="s">
+      <c r="Q6" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="R6" s="35" t="s">
+      <c r="R6" s="32" t="s">
         <v>18</v>
       </c>
       <c r="AA6"/>
@@ -3587,7 +3592,7 @@
       </c>
       <c r="F7" s="11">
         <f ca="1">F6/J26*J25</f>
-        <v>1409.090909090909</v>
+        <v>1972.7272727272725</v>
       </c>
       <c r="G7" s="11">
         <f ca="1">G6/J26*J25</f>
@@ -3597,7 +3602,7 @@
         <v>0</v>
       </c>
       <c r="J7" s="11">
-        <v>300</v>
+        <v>500</v>
       </c>
       <c r="L7" s="21">
         <v>0</v>
@@ -3605,19 +3610,19 @@
       <c r="M7" s="1">
         <v>299</v>
       </c>
-      <c r="N7" s="36">
+      <c r="N7" s="33">
         <v>300</v>
       </c>
-      <c r="O7" s="37">
+      <c r="O7" s="34">
         <v>300</v>
       </c>
-      <c r="P7" s="38">
+      <c r="P7" s="35">
         <v>300</v>
       </c>
-      <c r="Q7" s="39">
+      <c r="Q7" s="36">
         <v>300</v>
       </c>
-      <c r="R7" s="40">
+      <c r="R7" s="37">
         <v>300</v>
       </c>
       <c r="AB7" s="5"/>
@@ -3635,13 +3640,13 @@
       </c>
       <c r="F8" s="10">
         <f ca="1">F6/J26</f>
-        <v>45.454545454545453</v>
+        <v>63.636363636363633</v>
       </c>
       <c r="G8" s="10">
         <f ca="1">G6/J26</f>
         <v>45.454545454545453</v>
       </c>
-      <c r="I8" s="41" t="s">
+      <c r="I8" s="38" t="s">
         <v>4</v>
       </c>
       <c r="J8" s="11">
@@ -3653,19 +3658,19 @@
       <c r="M8" s="1">
         <v>599</v>
       </c>
-      <c r="N8" s="36">
+      <c r="N8" s="33">
         <v>100</v>
       </c>
-      <c r="O8" s="37">
+      <c r="O8" s="34">
         <v>150</v>
       </c>
-      <c r="P8" s="38">
+      <c r="P8" s="35">
         <v>200</v>
       </c>
-      <c r="Q8" s="39">
+      <c r="Q8" s="36">
         <v>250</v>
       </c>
-      <c r="R8" s="40">
+      <c r="R8" s="37">
         <v>300</v>
       </c>
     </row>
@@ -3688,11 +3693,11 @@
         <f ca="1">50*J27 + IF(J25&lt;30,(30-J25)*G8,0)</f>
         <v>1000</v>
       </c>
-      <c r="I9" s="41" t="s">
+      <c r="I9" s="38" t="s">
         <v>27</v>
       </c>
       <c r="J9" s="11">
-        <v>220</v>
+        <v>266</v>
       </c>
       <c r="L9" s="21">
         <v>600</v>
@@ -3700,19 +3705,19 @@
       <c r="M9" s="1">
         <v>899</v>
       </c>
-      <c r="N9" s="36">
+      <c r="N9" s="33">
         <v>75</v>
       </c>
-      <c r="O9" s="37">
+      <c r="O9" s="34">
         <v>100</v>
       </c>
-      <c r="P9" s="38">
+      <c r="P9" s="35">
         <v>150</v>
       </c>
-      <c r="Q9" s="39">
+      <c r="Q9" s="36">
         <v>200</v>
       </c>
-      <c r="R9" s="40">
+      <c r="R9" s="37">
         <v>300</v>
       </c>
     </row>
@@ -3725,10 +3730,10 @@
         <v>300</v>
       </c>
       <c r="E10" s="12"/>
-      <c r="I10" s="41" t="s">
+      <c r="I10" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="J10" s="41">
+      <c r="J10" s="38">
         <v>300</v>
       </c>
       <c r="L10" s="21">
@@ -3737,19 +3742,19 @@
       <c r="M10" s="1">
         <v>1199</v>
       </c>
-      <c r="N10" s="36">
+      <c r="N10" s="33">
         <v>50</v>
       </c>
-      <c r="O10" s="37">
+      <c r="O10" s="34">
         <v>75</v>
       </c>
-      <c r="P10" s="38">
+      <c r="P10" s="35">
         <v>100</v>
       </c>
-      <c r="Q10" s="39">
+      <c r="Q10" s="36">
         <v>175</v>
       </c>
-      <c r="R10" s="40">
+      <c r="R10" s="37">
         <v>300</v>
       </c>
     </row>
@@ -3761,16 +3766,16 @@
         <f ca="1">SUM(C6:C10)</f>
         <v>2700</v>
       </c>
-      <c r="E11" s="42" t="s">
+      <c r="E11" s="67" t="s">
         <v>27</v>
       </c>
-      <c r="F11" s="43"/>
-      <c r="G11" s="44"/>
-      <c r="I11" s="41" t="s">
+      <c r="F11" s="68"/>
+      <c r="G11" s="69"/>
+      <c r="I11" s="38" t="s">
         <v>44</v>
       </c>
       <c r="J11" s="11">
-        <v>800</v>
+        <v>700</v>
       </c>
       <c r="L11" s="21">
         <v>1200</v>
@@ -3778,19 +3783,19 @@
       <c r="M11" s="1">
         <v>1499</v>
       </c>
-      <c r="N11" s="36">
+      <c r="N11" s="33">
         <v>25</v>
       </c>
-      <c r="O11" s="37">
+      <c r="O11" s="34">
         <v>50</v>
       </c>
-      <c r="P11" s="38">
+      <c r="P11" s="35">
         <v>75</v>
       </c>
-      <c r="Q11" s="39">
+      <c r="Q11" s="36">
         <v>125</v>
       </c>
-      <c r="R11" s="40">
+      <c r="R11" s="37">
         <v>300</v>
       </c>
       <c r="Z11"/>
@@ -3804,19 +3809,19 @@
         <v>Diamond</v>
       </c>
       <c r="D12" s="5"/>
-      <c r="E12" s="26" t="s">
+      <c r="E12" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="F12" s="27" t="s">
+      <c r="F12" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="G12" s="26" t="s">
+      <c r="G12" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="I12" s="41" t="s">
+      <c r="I12" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="J12" s="41">
+      <c r="J12" s="38">
         <v>300</v>
       </c>
       <c r="L12" s="21">
@@ -3825,19 +3830,19 @@
       <c r="M12" s="1">
         <v>1799</v>
       </c>
-      <c r="N12" s="36">
+      <c r="N12" s="33">
         <v>10</v>
       </c>
-      <c r="O12" s="37">
+      <c r="O12" s="34">
         <v>25</v>
       </c>
-      <c r="P12" s="38">
+      <c r="P12" s="35">
         <v>50</v>
       </c>
-      <c r="Q12" s="39">
+      <c r="Q12" s="36">
         <v>100</v>
       </c>
-      <c r="R12" s="40">
+      <c r="R12" s="37">
         <v>250</v>
       </c>
       <c r="T12" s="4"/>
@@ -3847,7 +3852,7 @@
       <c r="B13" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="45" t="b">
+      <c r="C13" s="39" t="b">
         <v>0</v>
       </c>
       <c r="E13" s="1">
@@ -3861,11 +3866,11 @@
         <f>NightTimeDrive1114[[#This Row],[Penalty Weight]]*NightTimeDrive1114[[#This Row],[Duration]]</f>
         <v>0</v>
       </c>
-      <c r="I13" s="41" t="s">
+      <c r="I13" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="J13" s="41">
-        <v>2000</v>
+      <c r="J13" s="38">
+        <v>1500</v>
       </c>
       <c r="L13" s="22">
         <v>1800</v>
@@ -3873,19 +3878,19 @@
       <c r="M13" s="20">
         <v>1800</v>
       </c>
-      <c r="N13" s="46">
+      <c r="N13" s="40">
         <v>5</v>
       </c>
-      <c r="O13" s="47">
+      <c r="O13" s="41">
         <v>10</v>
       </c>
-      <c r="P13" s="48">
+      <c r="P13" s="42">
         <v>25</v>
       </c>
-      <c r="Q13" s="49">
+      <c r="Q13" s="43">
         <v>60</v>
       </c>
-      <c r="R13" s="50">
+      <c r="R13" s="44">
         <v>100</v>
       </c>
       <c r="W13"/>
@@ -3896,9 +3901,9 @@
       <c r="B14" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="51">
+      <c r="C14" s="45">
         <f>J13</f>
-        <v>2000</v>
+        <v>1500</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>47</v>
@@ -3927,17 +3932,17 @@
       <c r="B15" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="52" t="str">
+      <c r="C15" s="46" t="str">
         <f ca="1">_xlfn.CONCAT("Đ",J31*VLOOKUP(C12,O26:P31,2,FALSE)*10)</f>
-        <v>Đ10000</v>
+        <v>Đ7500</v>
       </c>
       <c r="D15" s="6"/>
-      <c r="N15" s="42" t="str">
+      <c r="N15" s="67" t="str">
         <f>_xlfn.CONCAT("Distance Points for ",J14)</f>
         <v>Distance Points for Diamond</v>
       </c>
-      <c r="O15" s="43"/>
-      <c r="P15" s="44"/>
+      <c r="O15" s="68"/>
+      <c r="P15" s="69"/>
       <c r="T15"/>
       <c r="U15"/>
       <c r="V15" s="18"/>
@@ -3950,21 +3955,21 @@
       <c r="B16" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C16" s="51">
+      <c r="C16" s="45">
         <f ca="1">MAX(0,C11-C14)</f>
-        <v>700</v>
-      </c>
-      <c r="I16" s="29" t="s">
+        <v>1200</v>
+      </c>
+      <c r="I16" s="64" t="s">
         <v>38</v>
       </c>
-      <c r="J16" s="29"/>
-      <c r="N16" s="28" t="s">
+      <c r="J16" s="64"/>
+      <c r="N16" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="O16" s="28" t="s">
+      <c r="O16" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="P16" s="28" t="s">
+      <c r="P16" s="26" t="s">
         <v>2</v>
       </c>
       <c r="T16"/>
@@ -3973,10 +3978,10 @@
     </row>
     <row r="17" spans="2:28" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H17" s="16"/>
-      <c r="I17" s="28" t="s">
+      <c r="I17" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="J17" s="28" t="s">
+      <c r="J17" s="26" t="s">
         <v>31</v>
       </c>
       <c r="N17" s="1" cm="1">
@@ -4057,10 +4062,10 @@
     </row>
     <row r="21" spans="2:28" x14ac:dyDescent="0.25">
       <c r="D21" s="16"/>
-      <c r="I21" s="29" t="s">
+      <c r="I21" s="64" t="s">
         <v>29</v>
       </c>
-      <c r="J21" s="29"/>
+      <c r="J21" s="64"/>
       <c r="N21" s="1">
         <v>1200</v>
       </c>
@@ -4079,10 +4084,10 @@
     </row>
     <row r="22" spans="2:28" x14ac:dyDescent="0.25">
       <c r="D22" s="16"/>
-      <c r="I22" s="28" t="s">
+      <c r="I22" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="J22" s="28" t="s">
+      <c r="J22" s="26" t="s">
         <v>31</v>
       </c>
       <c r="N22" s="1">
@@ -4150,13 +4155,13 @@
         <f ca="1">DAY(EOMONTH(TODAY(), 0))</f>
         <v>31</v>
       </c>
-      <c r="M25" s="29" t="s">
+      <c r="M25" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="N25" s="29"/>
-      <c r="O25" s="29"/>
-      <c r="P25" s="29"/>
-      <c r="Q25" s="29"/>
+      <c r="N25" s="64"/>
+      <c r="O25" s="64"/>
+      <c r="P25" s="64"/>
+      <c r="Q25" s="64"/>
       <c r="R25" s="3"/>
       <c r="T25"/>
       <c r="U25"/>
@@ -4175,19 +4180,19 @@
         <f ca="1">DAY(TODAY())-1</f>
         <v>11</v>
       </c>
-      <c r="M26" s="28" t="s">
+      <c r="M26" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="N26" s="28" t="s">
+      <c r="N26" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="O26" s="28" t="s">
+      <c r="O26" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="P26" s="28" t="s">
+      <c r="P26" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="Q26" s="28" t="s">
+      <c r="Q26" s="26" t="s">
         <v>49</v>
       </c>
       <c r="V26" s="2"/>
@@ -4203,19 +4208,19 @@
         <f ca="1">J25-J26</f>
         <v>20</v>
       </c>
-      <c r="M27" s="53">
+      <c r="M27" s="47">
         <v>0</v>
       </c>
-      <c r="N27" s="36">
+      <c r="N27" s="33">
         <v>799</v>
       </c>
-      <c r="O27" s="36" t="s">
+      <c r="O27" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="P27" s="54">
+      <c r="P27" s="48">
         <v>0.05</v>
       </c>
-      <c r="Q27" s="55" t="s">
+      <c r="Q27" s="49" t="s">
         <v>50</v>
       </c>
       <c r="T27" s="4"/>
@@ -4232,19 +4237,19 @@
         <f ca="1">C11-VLOOKUP(C11,M27:O31,1,TRUE)</f>
         <v>200</v>
       </c>
-      <c r="M28" s="56">
+      <c r="M28" s="50">
         <v>800</v>
       </c>
-      <c r="N28" s="37">
+      <c r="N28" s="34">
         <v>1599</v>
       </c>
-      <c r="O28" s="37" t="s">
+      <c r="O28" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="P28" s="57">
+      <c r="P28" s="51">
         <v>0.1</v>
       </c>
-      <c r="Q28" s="58" t="s">
+      <c r="Q28" s="52" t="s">
         <v>51</v>
       </c>
       <c r="T28" s="4"/>
@@ -4261,19 +4266,19 @@
         <f ca="1">MAX(0,C9-J28)</f>
         <v>100</v>
       </c>
-      <c r="M29" s="59">
+      <c r="M29" s="53">
         <v>1600</v>
       </c>
-      <c r="N29" s="38">
+      <c r="N29" s="35">
         <v>2199</v>
       </c>
-      <c r="O29" s="38" t="s">
+      <c r="O29" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="P29" s="60">
+      <c r="P29" s="54">
         <v>0.2</v>
       </c>
-      <c r="Q29" s="61" t="s">
+      <c r="Q29" s="55" t="s">
         <v>52</v>
       </c>
       <c r="T29" s="4"/>
@@ -4290,19 +4295,19 @@
         <f t="array" aca="1" ref="J30" ca="1">MAX(_xlfn._xlws.FILTER(_xlfn.ANCHORARRAY(O17),_xlfn.ANCHORARRAY( P17)&gt;=J29))</f>
         <v>1800</v>
       </c>
-      <c r="M30" s="62">
+      <c r="M30" s="56">
         <v>2200</v>
       </c>
-      <c r="N30" s="63">
+      <c r="N30" s="57">
         <v>2499</v>
       </c>
-      <c r="O30" s="63" t="s">
+      <c r="O30" s="57" t="s">
         <v>17</v>
       </c>
-      <c r="P30" s="64">
+      <c r="P30" s="58">
         <v>0.35</v>
       </c>
-      <c r="Q30" s="65" t="s">
+      <c r="Q30" s="59" t="s">
         <v>53</v>
       </c>
       <c r="T30" s="4"/>
@@ -4318,21 +4323,21 @@
       </c>
       <c r="J31" s="11">
         <f ca="1">MIN(C14,C11)</f>
-        <v>2000</v>
-      </c>
-      <c r="M31" s="66">
+        <v>1500</v>
+      </c>
+      <c r="M31" s="60">
         <v>2500</v>
       </c>
-      <c r="N31" s="67">
+      <c r="N31" s="61">
         <v>3000</v>
       </c>
-      <c r="O31" s="67" t="s">
+      <c r="O31" s="61" t="s">
         <v>18</v>
       </c>
-      <c r="P31" s="68">
+      <c r="P31" s="62">
         <v>0.5</v>
       </c>
-      <c r="Q31" s="69" t="s">
+      <c r="Q31" s="63" t="s">
         <v>55</v>
       </c>
       <c r="T31" s="4"/>
@@ -4406,12 +4411,11 @@
     </row>
   </sheetData>
   <protectedRanges>
-    <protectedRange sqref="F6:G6 C7:C8 C10 C16 C14" name="RequiresInput_1"/>
+    <protectedRange sqref="C7:C8 C10 C16 C14" name="RequiresInput_1"/>
+    <protectedRange sqref="F6:G6" name="RequiresInput_1_1"/>
   </protectedRanges>
   <dataConsolidate/>
   <mergeCells count="9">
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="I21:J21"/>
     <mergeCell ref="M25:Q25"/>
     <mergeCell ref="B2:G3"/>
     <mergeCell ref="I5:J5"/>
@@ -4419,38 +4423,40 @@
     <mergeCell ref="AB5:AC5"/>
     <mergeCell ref="E11:G11"/>
     <mergeCell ref="N15:P15"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="I21:J21"/>
   </mergeCells>
   <conditionalFormatting sqref="B11:C12">
-    <cfRule type="expression" dxfId="42" priority="1">
+    <cfRule type="expression" dxfId="29" priority="1">
       <formula>$C$12="Blue"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="41" priority="2">
+    <cfRule type="expression" dxfId="28" priority="2">
       <formula>$C$12="Bronze"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="3">
+    <cfRule type="expression" dxfId="27" priority="3">
       <formula>$C$12="Silver"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="39" priority="4">
+    <cfRule type="expression" dxfId="26" priority="4">
       <formula>$C$12="Gold"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="38" priority="5">
+    <cfRule type="expression" dxfId="25" priority="5">
       <formula>$C$12="Diamond"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P17:P23">
-    <cfRule type="expression" dxfId="37" priority="6">
+    <cfRule type="expression" dxfId="24" priority="6">
       <formula>$J$14="Blue"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="7">
+    <cfRule type="expression" dxfId="23" priority="7">
       <formula>$J$14="Bronze"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="35" priority="8">
+    <cfRule type="expression" dxfId="22" priority="8">
       <formula>$J$14="Silver"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="9">
+    <cfRule type="expression" dxfId="21" priority="9">
       <formula>$J$14="Gold"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="10">
+    <cfRule type="expression" dxfId="20" priority="10">
       <formula>$J$14="Diamond"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4474,8 +4480,8 @@
   </sheetPr>
   <dimension ref="B2:AC50"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4505,59 +4511,59 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:29" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="24" t="str">
+      <c r="B2" s="65" t="str">
         <f ca="1">_xlfn.CONCAT("Drive Summary ",J18, " ",TEXT(TODAY(), "mmmm yyyy"))</f>
         <v>Drive Summary Christiaan March 2025</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="25"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="65"/>
+      <c r="G2" s="65"/>
+      <c r="H2" s="23"/>
     </row>
     <row r="3" spans="2:29" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="25"/>
+      <c r="B3" s="65"/>
+      <c r="C3" s="65"/>
+      <c r="D3" s="65"/>
+      <c r="E3" s="65"/>
+      <c r="F3" s="65"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="23"/>
     </row>
     <row r="5" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B5" s="26" t="s">
+      <c r="B5" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="27" t="s">
+      <c r="C5" s="25" t="s">
         <v>31</v>
       </c>
       <c r="D5"/>
-      <c r="E5" s="26" t="str">
+      <c r="E5" s="24" t="str">
         <f ca="1">TEXT(TODAY(), "mmmm yyyy")</f>
         <v>March 2025</v>
       </c>
-      <c r="F5" s="26" t="s">
+      <c r="F5" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="G5" s="28" t="s">
+      <c r="G5" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="I5" s="29" t="s">
+      <c r="I5" s="64" t="s">
         <v>28</v>
       </c>
-      <c r="J5" s="29"/>
-      <c r="L5" s="29" t="s">
+      <c r="J5" s="64"/>
+      <c r="L5" s="64" t="s">
         <v>11</v>
       </c>
-      <c r="M5" s="29"/>
-      <c r="N5" s="29"/>
-      <c r="O5" s="29"/>
-      <c r="P5" s="29"/>
-      <c r="Q5" s="29"/>
-      <c r="R5" s="29"/>
-      <c r="AB5" s="23"/>
-      <c r="AC5" s="23"/>
+      <c r="M5" s="64"/>
+      <c r="N5" s="64"/>
+      <c r="O5" s="64"/>
+      <c r="P5" s="64"/>
+      <c r="Q5" s="64"/>
+      <c r="R5" s="64"/>
+      <c r="AB5" s="66"/>
+      <c r="AC5" s="66"/>
     </row>
     <row r="6" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
@@ -4570,37 +4576,39 @@
       <c r="E6" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F6" s="1">
-        <v>500</v>
-      </c>
-      <c r="G6" s="30">
-        <v>500</v>
-      </c>
-      <c r="I6" s="28" t="s">
+      <c r="F6" s="11">
+        <f>J11</f>
+        <v>0</v>
+      </c>
+      <c r="G6" s="27">
+        <f>J7</f>
+        <v>547</v>
+      </c>
+      <c r="I6" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="J6" s="28" t="s">
+      <c r="J6" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="L6" s="28" t="s">
+      <c r="L6" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="M6" s="28" t="s">
+      <c r="M6" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="N6" s="31" t="s">
+      <c r="N6" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="O6" s="32" t="s">
+      <c r="O6" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="P6" s="33" t="s">
+      <c r="P6" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="Q6" s="34" t="s">
+      <c r="Q6" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="R6" s="35" t="s">
+      <c r="R6" s="32" t="s">
         <v>18</v>
       </c>
       <c r="AA6"/>
@@ -4613,7 +4621,7 @@
       </c>
       <c r="C7" s="11">
         <f>J8</f>
-        <v>300</v>
+        <v>150</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="1" t="s">
@@ -4621,17 +4629,17 @@
       </c>
       <c r="F7" s="11">
         <f ca="1">F6/J26*J25</f>
-        <v>1409.090909090909</v>
+        <v>0</v>
       </c>
       <c r="G7" s="11">
         <f ca="1">G6/J26*J25</f>
-        <v>1409.090909090909</v>
+        <v>1541.5454545454545</v>
       </c>
       <c r="I7" s="11" t="s">
         <v>0</v>
       </c>
       <c r="J7" s="11">
-        <v>300</v>
+        <v>547</v>
       </c>
       <c r="L7" s="21">
         <v>0</v>
@@ -4639,19 +4647,19 @@
       <c r="M7" s="1">
         <v>299</v>
       </c>
-      <c r="N7" s="36">
+      <c r="N7" s="33">
         <v>300</v>
       </c>
-      <c r="O7" s="37">
+      <c r="O7" s="34">
         <v>300</v>
       </c>
-      <c r="P7" s="38">
+      <c r="P7" s="35">
         <v>300</v>
       </c>
-      <c r="Q7" s="39">
+      <c r="Q7" s="36">
         <v>300</v>
       </c>
-      <c r="R7" s="40">
+      <c r="R7" s="37">
         <v>300</v>
       </c>
       <c r="AB7" s="5"/>
@@ -4669,17 +4677,17 @@
       </c>
       <c r="F8" s="10">
         <f ca="1">F6/J26</f>
-        <v>45.454545454545453</v>
+        <v>0</v>
       </c>
       <c r="G8" s="10">
         <f ca="1">G6/J26</f>
-        <v>45.454545454545453</v>
-      </c>
-      <c r="I8" s="41" t="s">
+        <v>49.727272727272727</v>
+      </c>
+      <c r="I8" s="38" t="s">
         <v>4</v>
       </c>
       <c r="J8" s="11">
-        <v>300</v>
+        <v>150</v>
       </c>
       <c r="L8" s="21">
         <v>300</v>
@@ -4687,19 +4695,19 @@
       <c r="M8" s="1">
         <v>599</v>
       </c>
-      <c r="N8" s="36">
+      <c r="N8" s="33">
         <v>100</v>
       </c>
-      <c r="O8" s="37">
+      <c r="O8" s="34">
         <v>150</v>
       </c>
-      <c r="P8" s="38">
+      <c r="P8" s="35">
         <v>200</v>
       </c>
-      <c r="Q8" s="39">
+      <c r="Q8" s="36">
         <v>250</v>
       </c>
-      <c r="R8" s="40">
+      <c r="R8" s="37">
         <v>300</v>
       </c>
     </row>
@@ -4709,24 +4717,24 @@
       </c>
       <c r="C9" s="11">
         <f>VLOOKUP(IF(C13,F7,F6),N17:P23,3)</f>
-        <v>100</v>
+        <v>300</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>21</v>
       </c>
       <c r="F9" s="11">
         <f ca="1">IF(J30&gt;=M13, "Unlimited", J30-F6)</f>
-        <v>99</v>
+        <v>599</v>
       </c>
       <c r="G9" s="11">
         <f ca="1">50*J27 + IF(J25&lt;30,(30-J25)*G8,0)</f>
         <v>1000</v>
       </c>
-      <c r="I9" s="41" t="s">
+      <c r="I9" s="38" t="s">
         <v>27</v>
       </c>
       <c r="J9" s="11">
-        <v>220</v>
+        <v>300</v>
       </c>
       <c r="L9" s="21">
         <v>600</v>
@@ -4734,19 +4742,19 @@
       <c r="M9" s="1">
         <v>899</v>
       </c>
-      <c r="N9" s="36">
+      <c r="N9" s="33">
         <v>75</v>
       </c>
-      <c r="O9" s="37">
+      <c r="O9" s="34">
         <v>100</v>
       </c>
-      <c r="P9" s="38">
+      <c r="P9" s="35">
         <v>150</v>
       </c>
-      <c r="Q9" s="39">
+      <c r="Q9" s="36">
         <v>200</v>
       </c>
-      <c r="R9" s="40">
+      <c r="R9" s="37">
         <v>300</v>
       </c>
     </row>
@@ -4759,11 +4767,11 @@
         <v>300</v>
       </c>
       <c r="E10" s="12"/>
-      <c r="I10" s="41" t="s">
+      <c r="I10" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="J10" s="41">
-        <v>300</v>
+      <c r="J10" s="38">
+        <v>60</v>
       </c>
       <c r="L10" s="21">
         <v>900</v>
@@ -4771,19 +4779,19 @@
       <c r="M10" s="1">
         <v>1199</v>
       </c>
-      <c r="N10" s="36">
+      <c r="N10" s="33">
         <v>50</v>
       </c>
-      <c r="O10" s="37">
+      <c r="O10" s="34">
         <v>75</v>
       </c>
-      <c r="P10" s="38">
+      <c r="P10" s="35">
         <v>100</v>
       </c>
-      <c r="Q10" s="39">
+      <c r="Q10" s="36">
         <v>175</v>
       </c>
-      <c r="R10" s="40">
+      <c r="R10" s="37">
         <v>300</v>
       </c>
     </row>
@@ -4793,38 +4801,36 @@
       </c>
       <c r="C11" s="11">
         <f ca="1">SUM(C6:C10)</f>
-        <v>2500</v>
-      </c>
-      <c r="E11" s="42" t="s">
+        <v>2550</v>
+      </c>
+      <c r="E11" s="67" t="s">
         <v>27</v>
       </c>
-      <c r="F11" s="43"/>
-      <c r="G11" s="44"/>
-      <c r="I11" s="41" t="s">
+      <c r="F11" s="68"/>
+      <c r="G11" s="69"/>
+      <c r="I11" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="J11" s="11">
-        <v>800</v>
-      </c>
+      <c r="J11" s="11"/>
       <c r="L11" s="21">
         <v>1200</v>
       </c>
       <c r="M11" s="1">
         <v>1499</v>
       </c>
-      <c r="N11" s="36">
+      <c r="N11" s="33">
         <v>25</v>
       </c>
-      <c r="O11" s="37">
+      <c r="O11" s="34">
         <v>50</v>
       </c>
-      <c r="P11" s="38">
+      <c r="P11" s="35">
         <v>75</v>
       </c>
-      <c r="Q11" s="39">
+      <c r="Q11" s="36">
         <v>125</v>
       </c>
-      <c r="R11" s="40">
+      <c r="R11" s="37">
         <v>300</v>
       </c>
       <c r="Z11"/>
@@ -4838,19 +4844,19 @@
         <v>Diamond</v>
       </c>
       <c r="D12" s="5"/>
-      <c r="E12" s="26" t="s">
+      <c r="E12" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="F12" s="27" t="s">
+      <c r="F12" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="G12" s="26" t="s">
+      <c r="G12" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="I12" s="41" t="s">
+      <c r="I12" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="J12" s="41">
+      <c r="J12" s="38">
         <v>300</v>
       </c>
       <c r="L12" s="21">
@@ -4859,19 +4865,19 @@
       <c r="M12" s="1">
         <v>1799</v>
       </c>
-      <c r="N12" s="36">
+      <c r="N12" s="33">
         <v>10</v>
       </c>
-      <c r="O12" s="37">
+      <c r="O12" s="34">
         <v>25</v>
       </c>
-      <c r="P12" s="38">
+      <c r="P12" s="35">
         <v>50</v>
       </c>
-      <c r="Q12" s="39">
+      <c r="Q12" s="36">
         <v>100</v>
       </c>
-      <c r="R12" s="40">
+      <c r="R12" s="37">
         <v>250</v>
       </c>
       <c r="T12" s="4"/>
@@ -4881,7 +4887,7 @@
       <c r="B13" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="45" t="b">
+      <c r="C13" s="39" t="b">
         <v>0</v>
       </c>
       <c r="E13" s="1">
@@ -4895,11 +4901,11 @@
         <f>NightTimeDrive[[#This Row],[Penalty Weight]]*NightTimeDrive[[#This Row],[Duration]]</f>
         <v>0</v>
       </c>
-      <c r="I13" s="41" t="s">
+      <c r="I13" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="J13" s="41">
-        <v>2000</v>
+      <c r="J13" s="38">
+        <v>0</v>
       </c>
       <c r="L13" s="22">
         <v>1800</v>
@@ -4907,19 +4913,19 @@
       <c r="M13" s="20">
         <v>1800</v>
       </c>
-      <c r="N13" s="46">
+      <c r="N13" s="40">
         <v>5</v>
       </c>
-      <c r="O13" s="47">
+      <c r="O13" s="41">
         <v>10</v>
       </c>
-      <c r="P13" s="48">
+      <c r="P13" s="42">
         <v>25</v>
       </c>
-      <c r="Q13" s="49">
+      <c r="Q13" s="43">
         <v>60</v>
       </c>
-      <c r="R13" s="50">
+      <c r="R13" s="44">
         <v>100</v>
       </c>
       <c r="W13"/>
@@ -4930,9 +4936,9 @@
       <c r="B14" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="51">
+      <c r="C14" s="45">
         <f>J13</f>
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>47</v>
@@ -4949,7 +4955,7 @@
         <v>37</v>
       </c>
       <c r="J14" s="11" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="T14"/>
       <c r="U14"/>
@@ -4961,17 +4967,17 @@
       <c r="B15" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="52" t="str">
+      <c r="C15" s="46" t="str">
         <f ca="1">_xlfn.CONCAT("Đ",J31*VLOOKUP(C12,O26:P31,2,FALSE)*10)</f>
-        <v>Đ10000</v>
+        <v>Đ0</v>
       </c>
       <c r="D15" s="6"/>
-      <c r="N15" s="42" t="str">
+      <c r="N15" s="67" t="str">
         <f>_xlfn.CONCAT("Distance Points for ",J14)</f>
-        <v>Distance Points for Blue</v>
-      </c>
-      <c r="O15" s="43"/>
-      <c r="P15" s="44"/>
+        <v>Distance Points for Gold</v>
+      </c>
+      <c r="O15" s="68"/>
+      <c r="P15" s="69"/>
       <c r="T15"/>
       <c r="U15"/>
       <c r="V15" s="18"/>
@@ -4984,21 +4990,21 @@
       <c r="B16" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C16" s="51">
+      <c r="C16" s="45">
         <f ca="1">MAX(0,C11-C14)</f>
-        <v>500</v>
-      </c>
-      <c r="I16" s="29" t="s">
+        <v>2550</v>
+      </c>
+      <c r="I16" s="64" t="s">
         <v>38</v>
       </c>
-      <c r="J16" s="29"/>
-      <c r="N16" s="28" t="s">
+      <c r="J16" s="64"/>
+      <c r="N16" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="O16" s="28" t="s">
+      <c r="O16" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="P16" s="28" t="s">
+      <c r="P16" s="26" t="s">
         <v>2</v>
       </c>
       <c r="T16"/>
@@ -5007,10 +5013,10 @@
     </row>
     <row r="17" spans="2:28" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H17" s="16"/>
-      <c r="I17" s="28" t="s">
+      <c r="I17" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="J17" s="28" t="s">
+      <c r="J17" s="26" t="s">
         <v>31</v>
       </c>
       <c r="N17" s="1" cm="1">
@@ -5045,7 +5051,7 @@
         <v>599</v>
       </c>
       <c r="P18" s="1">
-        <v>100</v>
+        <v>250</v>
       </c>
       <c r="T18"/>
       <c r="U18"/>
@@ -5067,7 +5073,7 @@
         <v>899</v>
       </c>
       <c r="P19" s="1">
-        <v>75</v>
+        <v>200</v>
       </c>
       <c r="T19"/>
       <c r="U19"/>
@@ -5083,7 +5089,7 @@
         <v>1199</v>
       </c>
       <c r="P20" s="1">
-        <v>50</v>
+        <v>175</v>
       </c>
       <c r="T20"/>
       <c r="V20"/>
@@ -5091,10 +5097,10 @@
     </row>
     <row r="21" spans="2:28" x14ac:dyDescent="0.25">
       <c r="D21" s="16"/>
-      <c r="I21" s="29" t="s">
+      <c r="I21" s="64" t="s">
         <v>29</v>
       </c>
-      <c r="J21" s="29"/>
+      <c r="J21" s="64"/>
       <c r="N21" s="1">
         <v>1200</v>
       </c>
@@ -5102,7 +5108,7 @@
         <v>1499</v>
       </c>
       <c r="P21" s="1">
-        <v>25</v>
+        <v>125</v>
       </c>
       <c r="T21"/>
       <c r="U21"/>
@@ -5113,10 +5119,10 @@
     </row>
     <row r="22" spans="2:28" x14ac:dyDescent="0.25">
       <c r="D22" s="16"/>
-      <c r="I22" s="28" t="s">
+      <c r="I22" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="J22" s="28" t="s">
+      <c r="J22" s="26" t="s">
         <v>31</v>
       </c>
       <c r="N22" s="1">
@@ -5126,7 +5132,7 @@
         <v>1799</v>
       </c>
       <c r="P22" s="1">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="AA22" s="5"/>
       <c r="AB22" s="5"/>
@@ -5148,7 +5154,7 @@
         <v>1800</v>
       </c>
       <c r="P23" s="1">
-        <v>5</v>
+        <v>60</v>
       </c>
       <c r="T23"/>
       <c r="U23"/>
@@ -5165,7 +5171,7 @@
       </c>
       <c r="J24" s="1" t="str">
         <f>IF( AND( J9&lt;=J23+J19, J9&gt;=J23-J19 ), "Extract", "Calculate")</f>
-        <v>Calculate</v>
+        <v>Extract</v>
       </c>
       <c r="T24"/>
       <c r="U24"/>
@@ -5184,13 +5190,13 @@
         <f ca="1">DAY(EOMONTH(TODAY(), 0))</f>
         <v>31</v>
       </c>
-      <c r="M25" s="29" t="s">
+      <c r="M25" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="N25" s="29"/>
-      <c r="O25" s="29"/>
-      <c r="P25" s="29"/>
-      <c r="Q25" s="29"/>
+      <c r="N25" s="64"/>
+      <c r="O25" s="64"/>
+      <c r="P25" s="64"/>
+      <c r="Q25" s="64"/>
       <c r="R25" s="3"/>
       <c r="T25"/>
       <c r="U25"/>
@@ -5209,19 +5215,19 @@
         <f ca="1">DAY(TODAY())-1</f>
         <v>11</v>
       </c>
-      <c r="M26" s="28" t="s">
+      <c r="M26" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="N26" s="28" t="s">
+      <c r="N26" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="O26" s="28" t="s">
+      <c r="O26" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="P26" s="28" t="s">
+      <c r="P26" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="Q26" s="28" t="s">
+      <c r="Q26" s="26" t="s">
         <v>49</v>
       </c>
       <c r="V26" s="2"/>
@@ -5237,19 +5243,19 @@
         <f ca="1">J25-J26</f>
         <v>20</v>
       </c>
-      <c r="M27" s="53">
+      <c r="M27" s="47">
         <v>0</v>
       </c>
-      <c r="N27" s="36">
+      <c r="N27" s="33">
         <v>799</v>
       </c>
-      <c r="O27" s="36" t="s">
+      <c r="O27" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="P27" s="54">
+      <c r="P27" s="48">
         <v>0.05</v>
       </c>
-      <c r="Q27" s="55" t="s">
+      <c r="Q27" s="49" t="s">
         <v>50</v>
       </c>
       <c r="T27" s="4"/>
@@ -5264,21 +5270,21 @@
       </c>
       <c r="J28" s="11">
         <f ca="1">C11-VLOOKUP(C11,M27:O31,1,TRUE)</f>
-        <v>0</v>
-      </c>
-      <c r="M28" s="56">
+        <v>50</v>
+      </c>
+      <c r="M28" s="50">
         <v>800</v>
       </c>
-      <c r="N28" s="37">
+      <c r="N28" s="34">
         <v>1599</v>
       </c>
-      <c r="O28" s="37" t="s">
+      <c r="O28" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="P28" s="57">
+      <c r="P28" s="51">
         <v>0.1</v>
       </c>
-      <c r="Q28" s="58" t="s">
+      <c r="Q28" s="52" t="s">
         <v>51</v>
       </c>
       <c r="T28" s="4"/>
@@ -5293,21 +5299,21 @@
       </c>
       <c r="J29" s="11">
         <f ca="1">MAX(0,C9-J28)</f>
-        <v>100</v>
-      </c>
-      <c r="M29" s="59">
+        <v>250</v>
+      </c>
+      <c r="M29" s="53">
         <v>1600</v>
       </c>
-      <c r="N29" s="38">
+      <c r="N29" s="35">
         <v>2199</v>
       </c>
-      <c r="O29" s="38" t="s">
+      <c r="O29" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="P29" s="60">
+      <c r="P29" s="54">
         <v>0.2</v>
       </c>
-      <c r="Q29" s="61" t="s">
+      <c r="Q29" s="55" t="s">
         <v>52</v>
       </c>
       <c r="T29" s="4"/>
@@ -5324,19 +5330,19 @@
         <f t="array" aca="1" ref="J30" ca="1">MAX(_xlfn._xlws.FILTER(_xlfn.ANCHORARRAY(O17),_xlfn.ANCHORARRAY( P17)&gt;=J29))</f>
         <v>599</v>
       </c>
-      <c r="M30" s="62">
+      <c r="M30" s="56">
         <v>2200</v>
       </c>
-      <c r="N30" s="63">
+      <c r="N30" s="57">
         <v>2499</v>
       </c>
-      <c r="O30" s="63" t="s">
+      <c r="O30" s="57" t="s">
         <v>17</v>
       </c>
-      <c r="P30" s="64">
+      <c r="P30" s="58">
         <v>0.35</v>
       </c>
-      <c r="Q30" s="65" t="s">
+      <c r="Q30" s="59" t="s">
         <v>53</v>
       </c>
       <c r="T30" s="4"/>
@@ -5352,21 +5358,21 @@
       </c>
       <c r="J31" s="11">
         <f ca="1">MIN(C14,C11)</f>
-        <v>2000</v>
-      </c>
-      <c r="M31" s="66">
+        <v>0</v>
+      </c>
+      <c r="M31" s="60">
         <v>2500</v>
       </c>
-      <c r="N31" s="67">
+      <c r="N31" s="61">
         <v>3000</v>
       </c>
-      <c r="O31" s="67" t="s">
+      <c r="O31" s="61" t="s">
         <v>18</v>
       </c>
-      <c r="P31" s="68">
+      <c r="P31" s="62">
         <v>0.5</v>
       </c>
-      <c r="Q31" s="69" t="s">
+      <c r="Q31" s="63" t="s">
         <v>55</v>
       </c>
       <c r="T31" s="4"/>
@@ -5444,8 +5450,6 @@
   </protectedRanges>
   <dataConsolidate/>
   <mergeCells count="9">
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="I21:J21"/>
     <mergeCell ref="M25:Q25"/>
     <mergeCell ref="B2:G3"/>
     <mergeCell ref="I5:J5"/>
@@ -5453,38 +5457,40 @@
     <mergeCell ref="AB5:AC5"/>
     <mergeCell ref="E11:G11"/>
     <mergeCell ref="N15:P15"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="I21:J21"/>
   </mergeCells>
   <conditionalFormatting sqref="B11:C12">
-    <cfRule type="expression" dxfId="128" priority="1">
+    <cfRule type="expression" dxfId="19" priority="1">
       <formula>$C$12="Blue"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="127" priority="2">
+    <cfRule type="expression" dxfId="18" priority="2">
       <formula>$C$12="Bronze"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="126" priority="3">
+    <cfRule type="expression" dxfId="17" priority="3">
       <formula>$C$12="Silver"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="125" priority="4">
+    <cfRule type="expression" dxfId="16" priority="4">
       <formula>$C$12="Gold"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="124" priority="5">
+    <cfRule type="expression" dxfId="15" priority="5">
       <formula>$C$12="Diamond"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P17:P23">
-    <cfRule type="expression" dxfId="123" priority="6">
+    <cfRule type="expression" dxfId="14" priority="6">
       <formula>$J$14="Blue"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="122" priority="7">
+    <cfRule type="expression" dxfId="13" priority="7">
       <formula>$J$14="Bronze"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="121" priority="8">
+    <cfRule type="expression" dxfId="12" priority="8">
       <formula>$J$14="Silver"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="120" priority="9">
+    <cfRule type="expression" dxfId="11" priority="9">
       <formula>$J$14="Gold"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="119" priority="10">
+    <cfRule type="expression" dxfId="10" priority="10">
       <formula>$J$14="Diamond"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5508,8 +5514,8 @@
   </sheetPr>
   <dimension ref="B2:AC50"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5539,59 +5545,59 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:29" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="24" t="str">
+      <c r="B2" s="65" t="str">
         <f ca="1">_xlfn.CONCAT("Drive Summary ",J18, " ",TEXT(TODAY(), "mmmm yyyy"))</f>
         <v>Drive Summary Derrick March 2025</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="25"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="65"/>
+      <c r="G2" s="65"/>
+      <c r="H2" s="23"/>
     </row>
     <row r="3" spans="2:29" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="25"/>
+      <c r="B3" s="65"/>
+      <c r="C3" s="65"/>
+      <c r="D3" s="65"/>
+      <c r="E3" s="65"/>
+      <c r="F3" s="65"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="23"/>
     </row>
     <row r="5" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B5" s="26" t="s">
+      <c r="B5" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="27" t="s">
+      <c r="C5" s="25" t="s">
         <v>31</v>
       </c>
       <c r="D5"/>
-      <c r="E5" s="26" t="str">
+      <c r="E5" s="24" t="str">
         <f ca="1">TEXT(TODAY(), "mmmm yyyy")</f>
         <v>March 2025</v>
       </c>
-      <c r="F5" s="26" t="s">
+      <c r="F5" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="G5" s="28" t="s">
+      <c r="G5" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="I5" s="29" t="s">
+      <c r="I5" s="64" t="s">
         <v>28</v>
       </c>
-      <c r="J5" s="29"/>
-      <c r="L5" s="29" t="s">
+      <c r="J5" s="64"/>
+      <c r="L5" s="64" t="s">
         <v>11</v>
       </c>
-      <c r="M5" s="29"/>
-      <c r="N5" s="29"/>
-      <c r="O5" s="29"/>
-      <c r="P5" s="29"/>
-      <c r="Q5" s="29"/>
-      <c r="R5" s="29"/>
-      <c r="AB5" s="23"/>
-      <c r="AC5" s="23"/>
+      <c r="M5" s="64"/>
+      <c r="N5" s="64"/>
+      <c r="O5" s="64"/>
+      <c r="P5" s="64"/>
+      <c r="Q5" s="64"/>
+      <c r="R5" s="64"/>
+      <c r="AB5" s="66"/>
+      <c r="AC5" s="66"/>
     </row>
     <row r="6" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
@@ -5604,37 +5610,39 @@
       <c r="E6" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F6" s="1">
-        <v>500</v>
-      </c>
-      <c r="G6" s="30">
-        <v>500</v>
-      </c>
-      <c r="I6" s="28" t="s">
+      <c r="F6" s="11">
+        <f>J11</f>
+        <v>215</v>
+      </c>
+      <c r="G6" s="27">
+        <f>J7</f>
+        <v>549</v>
+      </c>
+      <c r="I6" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="J6" s="28" t="s">
+      <c r="J6" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="L6" s="28" t="s">
+      <c r="L6" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="M6" s="28" t="s">
+      <c r="M6" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="N6" s="31" t="s">
+      <c r="N6" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="O6" s="32" t="s">
+      <c r="O6" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="P6" s="33" t="s">
+      <c r="P6" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="Q6" s="34" t="s">
+      <c r="Q6" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="R6" s="35" t="s">
+      <c r="R6" s="32" t="s">
         <v>18</v>
       </c>
       <c r="AA6"/>
@@ -5647,7 +5655,7 @@
       </c>
       <c r="C7" s="11">
         <f>J8</f>
-        <v>300</v>
+        <v>150</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="1" t="s">
@@ -5655,17 +5663,17 @@
       </c>
       <c r="F7" s="11">
         <f ca="1">F6/J26*J25</f>
-        <v>1409.090909090909</v>
+        <v>605.90909090909099</v>
       </c>
       <c r="G7" s="11">
         <f ca="1">G6/J26*J25</f>
-        <v>1409.090909090909</v>
+        <v>1547.181818181818</v>
       </c>
       <c r="I7" s="11" t="s">
         <v>0</v>
       </c>
       <c r="J7" s="11">
-        <v>300</v>
+        <v>549</v>
       </c>
       <c r="L7" s="21">
         <v>0</v>
@@ -5673,19 +5681,19 @@
       <c r="M7" s="1">
         <v>299</v>
       </c>
-      <c r="N7" s="36">
+      <c r="N7" s="33">
         <v>300</v>
       </c>
-      <c r="O7" s="37">
+      <c r="O7" s="34">
         <v>300</v>
       </c>
-      <c r="P7" s="38">
+      <c r="P7" s="35">
         <v>300</v>
       </c>
-      <c r="Q7" s="39">
+      <c r="Q7" s="36">
         <v>300</v>
       </c>
-      <c r="R7" s="40">
+      <c r="R7" s="37">
         <v>300</v>
       </c>
       <c r="AB7" s="5"/>
@@ -5703,17 +5711,17 @@
       </c>
       <c r="F8" s="10">
         <f ca="1">F6/J26</f>
-        <v>45.454545454545453</v>
+        <v>19.545454545454547</v>
       </c>
       <c r="G8" s="10">
         <f ca="1">G6/J26</f>
-        <v>45.454545454545453</v>
-      </c>
-      <c r="I8" s="41" t="s">
+        <v>49.909090909090907</v>
+      </c>
+      <c r="I8" s="38" t="s">
         <v>4</v>
       </c>
       <c r="J8" s="11">
-        <v>300</v>
+        <v>150</v>
       </c>
       <c r="L8" s="21">
         <v>300</v>
@@ -5721,19 +5729,19 @@
       <c r="M8" s="1">
         <v>599</v>
       </c>
-      <c r="N8" s="36">
+      <c r="N8" s="33">
         <v>100</v>
       </c>
-      <c r="O8" s="37">
+      <c r="O8" s="34">
         <v>150</v>
       </c>
-      <c r="P8" s="38">
+      <c r="P8" s="35">
         <v>200</v>
       </c>
-      <c r="Q8" s="39">
+      <c r="Q8" s="36">
         <v>250</v>
       </c>
-      <c r="R8" s="40">
+      <c r="R8" s="37">
         <v>300</v>
       </c>
     </row>
@@ -5743,24 +5751,24 @@
       </c>
       <c r="C9" s="11">
         <f>VLOOKUP(IF(C13,F7,F6),N17:P23,3)</f>
-        <v>100</v>
+        <v>300</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>21</v>
       </c>
       <c r="F9" s="11">
         <f ca="1">IF(J30&gt;=M13, "Unlimited", J30-F6)</f>
-        <v>99</v>
+        <v>384</v>
       </c>
       <c r="G9" s="11">
         <f ca="1">50*J27 + IF(J25&lt;30,(30-J25)*G8,0)</f>
         <v>1000</v>
       </c>
-      <c r="I9" s="41" t="s">
+      <c r="I9" s="38" t="s">
         <v>27</v>
       </c>
       <c r="J9" s="11">
-        <v>220</v>
+        <v>300</v>
       </c>
       <c r="L9" s="21">
         <v>600</v>
@@ -5768,19 +5776,19 @@
       <c r="M9" s="1">
         <v>899</v>
       </c>
-      <c r="N9" s="36">
+      <c r="N9" s="33">
         <v>75</v>
       </c>
-      <c r="O9" s="37">
+      <c r="O9" s="34">
         <v>100</v>
       </c>
-      <c r="P9" s="38">
+      <c r="P9" s="35">
         <v>150</v>
       </c>
-      <c r="Q9" s="39">
+      <c r="Q9" s="36">
         <v>200</v>
       </c>
-      <c r="R9" s="40">
+      <c r="R9" s="37">
         <v>300</v>
       </c>
     </row>
@@ -5793,11 +5801,11 @@
         <v>300</v>
       </c>
       <c r="E10" s="12"/>
-      <c r="I10" s="41" t="s">
+      <c r="I10" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="J10" s="41">
-        <v>300</v>
+      <c r="J10" s="38">
+        <v>200</v>
       </c>
       <c r="L10" s="21">
         <v>900</v>
@@ -5805,19 +5813,19 @@
       <c r="M10" s="1">
         <v>1199</v>
       </c>
-      <c r="N10" s="36">
+      <c r="N10" s="33">
         <v>50</v>
       </c>
-      <c r="O10" s="37">
+      <c r="O10" s="34">
         <v>75</v>
       </c>
-      <c r="P10" s="38">
+      <c r="P10" s="35">
         <v>100</v>
       </c>
-      <c r="Q10" s="39">
+      <c r="Q10" s="36">
         <v>175</v>
       </c>
-      <c r="R10" s="40">
+      <c r="R10" s="37">
         <v>300</v>
       </c>
     </row>
@@ -5827,18 +5835,18 @@
       </c>
       <c r="C11" s="11">
         <f ca="1">SUM(C6:C10)</f>
-        <v>2500</v>
-      </c>
-      <c r="E11" s="42" t="s">
+        <v>2550</v>
+      </c>
+      <c r="E11" s="67" t="s">
         <v>27</v>
       </c>
-      <c r="F11" s="43"/>
-      <c r="G11" s="44"/>
-      <c r="I11" s="41" t="s">
+      <c r="F11" s="68"/>
+      <c r="G11" s="69"/>
+      <c r="I11" s="38" t="s">
         <v>44</v>
       </c>
       <c r="J11" s="11">
-        <v>800</v>
+        <v>215</v>
       </c>
       <c r="L11" s="21">
         <v>1200</v>
@@ -5846,19 +5854,19 @@
       <c r="M11" s="1">
         <v>1499</v>
       </c>
-      <c r="N11" s="36">
+      <c r="N11" s="33">
         <v>25</v>
       </c>
-      <c r="O11" s="37">
+      <c r="O11" s="34">
         <v>50</v>
       </c>
-      <c r="P11" s="38">
+      <c r="P11" s="35">
         <v>75</v>
       </c>
-      <c r="Q11" s="39">
+      <c r="Q11" s="36">
         <v>125</v>
       </c>
-      <c r="R11" s="40">
+      <c r="R11" s="37">
         <v>300</v>
       </c>
       <c r="Z11"/>
@@ -5872,19 +5880,19 @@
         <v>Diamond</v>
       </c>
       <c r="D12" s="5"/>
-      <c r="E12" s="26" t="s">
+      <c r="E12" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="F12" s="27" t="s">
+      <c r="F12" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="G12" s="26" t="s">
+      <c r="G12" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="I12" s="41" t="s">
+      <c r="I12" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="J12" s="41">
+      <c r="J12" s="38">
         <v>300</v>
       </c>
       <c r="L12" s="21">
@@ -5893,19 +5901,19 @@
       <c r="M12" s="1">
         <v>1799</v>
       </c>
-      <c r="N12" s="36">
+      <c r="N12" s="33">
         <v>10</v>
       </c>
-      <c r="O12" s="37">
+      <c r="O12" s="34">
         <v>25</v>
       </c>
-      <c r="P12" s="38">
+      <c r="P12" s="35">
         <v>50</v>
       </c>
-      <c r="Q12" s="39">
+      <c r="Q12" s="36">
         <v>100</v>
       </c>
-      <c r="R12" s="40">
+      <c r="R12" s="37">
         <v>250</v>
       </c>
       <c r="T12" s="4"/>
@@ -5915,7 +5923,7 @@
       <c r="B13" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="45" t="b">
+      <c r="C13" s="39" t="b">
         <v>0</v>
       </c>
       <c r="E13" s="1">
@@ -5929,11 +5937,11 @@
         <f>NightTimeDrive11[[#This Row],[Penalty Weight]]*NightTimeDrive11[[#This Row],[Duration]]</f>
         <v>0</v>
       </c>
-      <c r="I13" s="41" t="s">
+      <c r="I13" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="J13" s="41">
-        <v>2000</v>
+      <c r="J13" s="38">
+        <v>0</v>
       </c>
       <c r="L13" s="22">
         <v>1800</v>
@@ -5941,19 +5949,19 @@
       <c r="M13" s="20">
         <v>1800</v>
       </c>
-      <c r="N13" s="46">
+      <c r="N13" s="40">
         <v>5</v>
       </c>
-      <c r="O13" s="47">
+      <c r="O13" s="41">
         <v>10</v>
       </c>
-      <c r="P13" s="48">
+      <c r="P13" s="42">
         <v>25</v>
       </c>
-      <c r="Q13" s="49">
+      <c r="Q13" s="43">
         <v>60</v>
       </c>
-      <c r="R13" s="50">
+      <c r="R13" s="44">
         <v>100</v>
       </c>
       <c r="W13"/>
@@ -5964,9 +5972,9 @@
       <c r="B14" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="51">
+      <c r="C14" s="45">
         <f>J13</f>
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>47</v>
@@ -5983,7 +5991,7 @@
         <v>37</v>
       </c>
       <c r="J14" s="11" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="T14"/>
       <c r="U14"/>
@@ -5995,17 +6003,17 @@
       <c r="B15" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="52" t="str">
+      <c r="C15" s="46" t="str">
         <f ca="1">_xlfn.CONCAT("Đ",J31*VLOOKUP(C12,O26:P31,2,FALSE)*10)</f>
-        <v>Đ10000</v>
+        <v>Đ0</v>
       </c>
       <c r="D15" s="6"/>
-      <c r="N15" s="42" t="str">
+      <c r="N15" s="67" t="str">
         <f>_xlfn.CONCAT("Distance Points for ",J14)</f>
-        <v>Distance Points for Blue</v>
-      </c>
-      <c r="O15" s="43"/>
-      <c r="P15" s="44"/>
+        <v>Distance Points for Gold</v>
+      </c>
+      <c r="O15" s="68"/>
+      <c r="P15" s="69"/>
       <c r="T15"/>
       <c r="U15"/>
       <c r="V15" s="18"/>
@@ -6018,21 +6026,21 @@
       <c r="B16" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C16" s="51">
+      <c r="C16" s="45">
         <f ca="1">MAX(0,C11-C14)</f>
-        <v>500</v>
-      </c>
-      <c r="I16" s="29" t="s">
+        <v>2550</v>
+      </c>
+      <c r="I16" s="64" t="s">
         <v>38</v>
       </c>
-      <c r="J16" s="29"/>
-      <c r="N16" s="28" t="s">
+      <c r="J16" s="64"/>
+      <c r="N16" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="O16" s="28" t="s">
+      <c r="O16" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="P16" s="28" t="s">
+      <c r="P16" s="26" t="s">
         <v>2</v>
       </c>
       <c r="T16"/>
@@ -6041,10 +6049,10 @@
     </row>
     <row r="17" spans="2:28" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H17" s="16"/>
-      <c r="I17" s="28" t="s">
+      <c r="I17" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="J17" s="28" t="s">
+      <c r="J17" s="26" t="s">
         <v>31</v>
       </c>
       <c r="N17" s="1" cm="1">
@@ -6079,7 +6087,7 @@
         <v>599</v>
       </c>
       <c r="P18" s="1">
-        <v>100</v>
+        <v>250</v>
       </c>
       <c r="T18"/>
       <c r="U18"/>
@@ -6101,7 +6109,7 @@
         <v>899</v>
       </c>
       <c r="P19" s="1">
-        <v>75</v>
+        <v>200</v>
       </c>
       <c r="T19"/>
       <c r="U19"/>
@@ -6117,7 +6125,7 @@
         <v>1199</v>
       </c>
       <c r="P20" s="1">
-        <v>50</v>
+        <v>175</v>
       </c>
       <c r="T20"/>
       <c r="V20"/>
@@ -6125,10 +6133,10 @@
     </row>
     <row r="21" spans="2:28" x14ac:dyDescent="0.25">
       <c r="D21" s="16"/>
-      <c r="I21" s="29" t="s">
+      <c r="I21" s="64" t="s">
         <v>29</v>
       </c>
-      <c r="J21" s="29"/>
+      <c r="J21" s="64"/>
       <c r="N21" s="1">
         <v>1200</v>
       </c>
@@ -6136,7 +6144,7 @@
         <v>1499</v>
       </c>
       <c r="P21" s="1">
-        <v>25</v>
+        <v>125</v>
       </c>
       <c r="T21"/>
       <c r="U21"/>
@@ -6147,10 +6155,10 @@
     </row>
     <row r="22" spans="2:28" x14ac:dyDescent="0.25">
       <c r="D22" s="16"/>
-      <c r="I22" s="28" t="s">
+      <c r="I22" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="J22" s="28" t="s">
+      <c r="J22" s="26" t="s">
         <v>31</v>
       </c>
       <c r="N22" s="1">
@@ -6160,7 +6168,7 @@
         <v>1799</v>
       </c>
       <c r="P22" s="1">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="AA22" s="5"/>
       <c r="AB22" s="5"/>
@@ -6182,7 +6190,7 @@
         <v>1800</v>
       </c>
       <c r="P23" s="1">
-        <v>5</v>
+        <v>60</v>
       </c>
       <c r="T23"/>
       <c r="U23"/>
@@ -6199,7 +6207,7 @@
       </c>
       <c r="J24" s="1" t="str">
         <f>IF( AND( J9&lt;=J23+J19, J9&gt;=J23-J19 ), "Extract", "Calculate")</f>
-        <v>Calculate</v>
+        <v>Extract</v>
       </c>
       <c r="T24"/>
       <c r="U24"/>
@@ -6218,13 +6226,13 @@
         <f ca="1">DAY(EOMONTH(TODAY(), 0))</f>
         <v>31</v>
       </c>
-      <c r="M25" s="29" t="s">
+      <c r="M25" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="N25" s="29"/>
-      <c r="O25" s="29"/>
-      <c r="P25" s="29"/>
-      <c r="Q25" s="29"/>
+      <c r="N25" s="64"/>
+      <c r="O25" s="64"/>
+      <c r="P25" s="64"/>
+      <c r="Q25" s="64"/>
       <c r="R25" s="3"/>
       <c r="T25"/>
       <c r="U25"/>
@@ -6243,19 +6251,19 @@
         <f ca="1">DAY(TODAY())-1</f>
         <v>11</v>
       </c>
-      <c r="M26" s="28" t="s">
+      <c r="M26" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="N26" s="28" t="s">
+      <c r="N26" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="O26" s="28" t="s">
+      <c r="O26" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="P26" s="28" t="s">
+      <c r="P26" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="Q26" s="28" t="s">
+      <c r="Q26" s="26" t="s">
         <v>49</v>
       </c>
       <c r="V26" s="2"/>
@@ -6271,19 +6279,19 @@
         <f ca="1">J25-J26</f>
         <v>20</v>
       </c>
-      <c r="M27" s="53">
+      <c r="M27" s="47">
         <v>0</v>
       </c>
-      <c r="N27" s="36">
+      <c r="N27" s="33">
         <v>799</v>
       </c>
-      <c r="O27" s="36" t="s">
+      <c r="O27" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="P27" s="54">
+      <c r="P27" s="48">
         <v>0.05</v>
       </c>
-      <c r="Q27" s="55" t="s">
+      <c r="Q27" s="49" t="s">
         <v>50</v>
       </c>
       <c r="T27" s="4"/>
@@ -6298,21 +6306,21 @@
       </c>
       <c r="J28" s="11">
         <f ca="1">C11-VLOOKUP(C11,M27:O31,1,TRUE)</f>
-        <v>0</v>
-      </c>
-      <c r="M28" s="56">
+        <v>50</v>
+      </c>
+      <c r="M28" s="50">
         <v>800</v>
       </c>
-      <c r="N28" s="37">
+      <c r="N28" s="34">
         <v>1599</v>
       </c>
-      <c r="O28" s="37" t="s">
+      <c r="O28" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="P28" s="57">
+      <c r="P28" s="51">
         <v>0.1</v>
       </c>
-      <c r="Q28" s="58" t="s">
+      <c r="Q28" s="52" t="s">
         <v>51</v>
       </c>
       <c r="T28" s="4"/>
@@ -6327,21 +6335,21 @@
       </c>
       <c r="J29" s="11">
         <f ca="1">MAX(0,C9-J28)</f>
-        <v>100</v>
-      </c>
-      <c r="M29" s="59">
+        <v>250</v>
+      </c>
+      <c r="M29" s="53">
         <v>1600</v>
       </c>
-      <c r="N29" s="38">
+      <c r="N29" s="35">
         <v>2199</v>
       </c>
-      <c r="O29" s="38" t="s">
+      <c r="O29" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="P29" s="60">
+      <c r="P29" s="54">
         <v>0.2</v>
       </c>
-      <c r="Q29" s="61" t="s">
+      <c r="Q29" s="55" t="s">
         <v>52</v>
       </c>
       <c r="T29" s="4"/>
@@ -6358,19 +6366,19 @@
         <f t="array" aca="1" ref="J30" ca="1">MAX(_xlfn._xlws.FILTER(_xlfn.ANCHORARRAY(O17),_xlfn.ANCHORARRAY( P17)&gt;=J29))</f>
         <v>599</v>
       </c>
-      <c r="M30" s="62">
+      <c r="M30" s="56">
         <v>2200</v>
       </c>
-      <c r="N30" s="63">
+      <c r="N30" s="57">
         <v>2499</v>
       </c>
-      <c r="O30" s="63" t="s">
+      <c r="O30" s="57" t="s">
         <v>17</v>
       </c>
-      <c r="P30" s="64">
+      <c r="P30" s="58">
         <v>0.35</v>
       </c>
-      <c r="Q30" s="65" t="s">
+      <c r="Q30" s="59" t="s">
         <v>53</v>
       </c>
       <c r="T30" s="4"/>
@@ -6386,21 +6394,21 @@
       </c>
       <c r="J31" s="11">
         <f ca="1">MIN(C14,C11)</f>
-        <v>2000</v>
-      </c>
-      <c r="M31" s="66">
+        <v>0</v>
+      </c>
+      <c r="M31" s="60">
         <v>2500</v>
       </c>
-      <c r="N31" s="67">
+      <c r="N31" s="61">
         <v>3000</v>
       </c>
-      <c r="O31" s="67" t="s">
+      <c r="O31" s="61" t="s">
         <v>18</v>
       </c>
-      <c r="P31" s="68">
+      <c r="P31" s="62">
         <v>0.5</v>
       </c>
-      <c r="Q31" s="69" t="s">
+      <c r="Q31" s="63" t="s">
         <v>55</v>
       </c>
       <c r="T31" s="4"/>
@@ -6474,12 +6482,11 @@
     </row>
   </sheetData>
   <protectedRanges>
-    <protectedRange sqref="F6:G6 C7:C8 C10 C16 C14" name="RequiresInput_1"/>
+    <protectedRange sqref="C7:C8 C10 C16 C14" name="RequiresInput_1"/>
+    <protectedRange sqref="F6:G6" name="RequiresInput_1_1"/>
   </protectedRanges>
   <dataConsolidate/>
   <mergeCells count="9">
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="I21:J21"/>
     <mergeCell ref="M25:Q25"/>
     <mergeCell ref="B2:G3"/>
     <mergeCell ref="I5:J5"/>
@@ -6487,38 +6494,40 @@
     <mergeCell ref="AB5:AC5"/>
     <mergeCell ref="E11:G11"/>
     <mergeCell ref="N15:P15"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="I21:J21"/>
   </mergeCells>
   <conditionalFormatting sqref="B11:C12">
-    <cfRule type="expression" dxfId="85" priority="1">
+    <cfRule type="expression" dxfId="9" priority="1">
       <formula>$C$12="Blue"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="84" priority="2">
+    <cfRule type="expression" dxfId="8" priority="2">
       <formula>$C$12="Bronze"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="83" priority="3">
+    <cfRule type="expression" dxfId="7" priority="3">
       <formula>$C$12="Silver"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="82" priority="4">
+    <cfRule type="expression" dxfId="6" priority="4">
       <formula>$C$12="Gold"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="81" priority="5">
+    <cfRule type="expression" dxfId="5" priority="5">
       <formula>$C$12="Diamond"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P17:P23">
-    <cfRule type="expression" dxfId="80" priority="6">
+    <cfRule type="expression" dxfId="4" priority="6">
       <formula>$J$14="Blue"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="79" priority="7">
+    <cfRule type="expression" dxfId="3" priority="7">
       <formula>$J$14="Bronze"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="78" priority="8">
+    <cfRule type="expression" dxfId="2" priority="8">
       <formula>$J$14="Silver"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="77" priority="9">
+    <cfRule type="expression" dxfId="1" priority="9">
       <formula>$J$14="Gold"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="76" priority="10">
+    <cfRule type="expression" dxfId="0" priority="10">
       <formula>$J$14="Diamond"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Started with Python Processing
</commit_message>
<xml_diff>
--- a/DriveSummary.xlsx
+++ b/DriveSummary.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2fd3bccd6dbaea2b/GitGud/ExcelDriveSummary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="13_ncr:1_{16BB77BC-72C4-43FD-98A0-25CDEB97D854}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D9DB8336-09AB-4C45-853E-8035CFDE224D}"/>
+  <xr:revisionPtr revIDLastSave="143" documentId="13_ncr:1_{16BB77BC-72C4-43FD-98A0-25CDEB97D854}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A6C7F1E4-81F2-42ED-91B0-37CB77B32663}"/>
   <bookViews>
-    <workbookView xWindow="-4140" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{B12B6E18-E294-4985-A977-422328ADD677}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{B12B6E18-E294-4985-A977-422328ADD677}"/>
   </bookViews>
   <sheets>
     <sheet name="Stefan" sheetId="20" r:id="rId1"/>
     <sheet name="Christiaan" sheetId="18" r:id="rId2"/>
-    <sheet name="Derrick" sheetId="19" r:id="rId3"/>
+    <sheet name="Derrick" sheetId="24" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="Username" localSheetId="1">Christiaan!$J$23</definedName>
@@ -780,7 +780,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Silver" xfId="3" xr:uid="{14E707C8-7A31-4C64-82D2-79D4451F1D93}"/>
   </cellStyles>
-  <dxfs count="131">
+  <dxfs count="145">
     <dxf>
       <fill>
         <patternFill>
@@ -2709,22 +2709,6 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
@@ -2764,22 +2748,6 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
@@ -2819,22 +2787,6 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
@@ -2993,7 +2945,7 @@
         <top style="thin">
           <color auto="1"/>
         </top>
-        <bottom style="thin">
+        <bottom style="medium">
           <color auto="1"/>
         </bottom>
         <vertical style="thin">
@@ -3004,12 +2956,432 @@
         </horizontal>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="medium">
+          <color auto="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="medium">
+          <color auto="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="medium">
+          <color auto="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="medium">
+          <color auto="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="medium">
+          <color auto="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="medium">
+          <color auto="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="medium">
+          <color auto="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="medium">
+          <color auto="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="medium">
+          <color auto="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="medium">
+          <color auto="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="medium">
+          <color auto="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="medium">
+          <color auto="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="medium">
+          <color auto="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
   </dxfs>
-  <tableStyles count="2" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+  <tableStyles count="16" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Table Style 1" pivot="0" count="1" xr9:uid="{A9F08CE5-ED7D-4BF0-BED4-1E9AB08F748B}">
+      <tableStyleElement type="wholeTable" dxfId="144"/>
+    </tableStyle>
+    <tableStyle name="Table Style 1 10" pivot="0" count="1" xr9:uid="{2D1C1F65-64AA-44E5-AA5A-2B6F13002934}">
+      <tableStyleElement type="wholeTable" dxfId="143"/>
+    </tableStyle>
+    <tableStyle name="Table Style 1 11" pivot="0" count="1" xr9:uid="{05AF31C5-0C6B-4FC9-BB2A-CC666AEEA938}">
+      <tableStyleElement type="wholeTable" dxfId="142"/>
+    </tableStyle>
+    <tableStyle name="Table Style 1 12" pivot="0" count="1" xr9:uid="{F7ADC423-0988-4DA8-B9D0-A07AA727111C}">
+      <tableStyleElement type="wholeTable" dxfId="141"/>
+    </tableStyle>
+    <tableStyle name="Table Style 1 13" pivot="0" count="1" xr9:uid="{DC96A2DC-53A1-4C21-A60E-F20A7120FF3C}">
+      <tableStyleElement type="wholeTable" dxfId="140"/>
+    </tableStyle>
+    <tableStyle name="Table Style 1 14" pivot="0" count="1" xr9:uid="{4681CA8B-13A2-463B-A4A2-F203979C6A14}">
+      <tableStyleElement type="wholeTable" dxfId="139"/>
+    </tableStyle>
+    <tableStyle name="Table Style 1 15" pivot="0" count="1" xr9:uid="{7B50F24D-1991-4972-9A49-6490DA20EE16}">
+      <tableStyleElement type="wholeTable" dxfId="138"/>
+    </tableStyle>
+    <tableStyle name="Table Style 1 16" pivot="0" count="1" xr9:uid="{CF2D3427-1AB2-4D49-B68E-B9C0B3EDBE75}">
+      <tableStyleElement type="wholeTable" dxfId="137"/>
+    </tableStyle>
+    <tableStyle name="Table Style 1 2" pivot="0" count="1" xr9:uid="{9328C6BF-6A18-40D6-BCF5-ACC71AF16E8E}">
+      <tableStyleElement type="wholeTable" dxfId="136"/>
+    </tableStyle>
+    <tableStyle name="Table Style 1 3" pivot="0" count="1" xr9:uid="{37EF096D-2DFE-477A-8568-8A16C87D899A}">
+      <tableStyleElement type="wholeTable" dxfId="135"/>
+    </tableStyle>
+    <tableStyle name="Table Style 1 4" pivot="0" count="1" xr9:uid="{8A7764C2-5FA0-4ED3-8FD1-B93D5D03E99F}">
+      <tableStyleElement type="wholeTable" dxfId="134"/>
+    </tableStyle>
+    <tableStyle name="Table Style 1 5" pivot="0" count="1" xr9:uid="{F304E450-A967-49C6-88DB-FE75A7950572}">
+      <tableStyleElement type="wholeTable" dxfId="133"/>
+    </tableStyle>
+    <tableStyle name="Table Style 1 6" pivot="0" count="1" xr9:uid="{0F2E8DB9-5B38-455C-8A1C-56B0099F7828}">
+      <tableStyleElement type="wholeTable" dxfId="132"/>
+    </tableStyle>
+    <tableStyle name="Table Style 1 7" pivot="0" count="1" xr9:uid="{3512C574-7CC4-49B4-A867-7F44CFB3F84B}">
+      <tableStyleElement type="wholeTable" dxfId="131"/>
+    </tableStyle>
+    <tableStyle name="Table Style 1 8" pivot="0" count="1" xr9:uid="{A7D82AA8-1F0A-4767-816C-D08C9223EDC9}">
       <tableStyleElement type="wholeTable" dxfId="130"/>
     </tableStyle>
-    <tableStyle name="Table Style 1 2" pivot="0" count="1" xr9:uid="{9328C6BF-6A18-40D6-BCF5-ACC71AF16E8E}">
+    <tableStyle name="Table Style 1 9" pivot="0" count="1" xr9:uid="{ED2ED81A-DDBA-4F91-A0D7-17E66D871F9A}">
       <tableStyleElement type="wholeTable" dxfId="129"/>
     </tableStyle>
   </tableStyles>
@@ -3041,20 +3413,22 @@
 </FeaturePropertyBags>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{52D41F9E-201D-494C-B741-54D3661AF0CB}" name="NightTimeDrive1114" displayName="NightTimeDrive1114" ref="E12:G14" totalsRowCount="1" headerRowDxfId="128" dataDxfId="126" totalsRowDxfId="124" headerRowBorderDxfId="127" tableBorderDxfId="125" totalsRowBorderDxfId="123">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{52D41F9E-201D-494C-B741-54D3661AF0CB}" name="NightTimeDriveStefan" displayName="NightTimeDriveStefan" ref="E12:G14" totalsRowCount="1" headerRowDxfId="128" dataDxfId="126" totalsRowDxfId="124" headerRowBorderDxfId="127" tableBorderDxfId="125" totalsRowBorderDxfId="123">
   <autoFilter ref="E12:G13" xr:uid="{932FCD99-6FCF-4AE6-A66E-74A568E6D121}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{E9820CD1-120D-416C-8D24-0E189A941AF9}" name="Penalty Weight" totalsRowLabel="Total" dataDxfId="122" totalsRowDxfId="121">
-      <calculatedColumnFormula>2</calculatedColumnFormula>
-    </tableColumn>
+    <tableColumn id="1" xr3:uid="{E9820CD1-120D-416C-8D24-0E189A941AF9}" name="Penalty Weight" totalsRowLabel="Total" dataDxfId="122" totalsRowDxfId="121"/>
     <tableColumn id="2" xr3:uid="{770CBEF7-6A21-4F31-A449-460FF496815E}" name="Duration" totalsRowFunction="sum" dataDxfId="120" totalsRowDxfId="119"/>
     <tableColumn id="3" xr3:uid="{16E6B1A8-A2A6-468A-8C73-0F393F4B41CE}" name="Points" totalsRowFunction="sum" dataDxfId="118" totalsRowDxfId="117">
-      <calculatedColumnFormula>NightTimeDrive1114[[#This Row],[Penalty Weight]]*NightTimeDrive1114[[#This Row],[Duration]]</calculatedColumnFormula>
+      <calculatedColumnFormula>NightTimeDriveStefan[[#This Row],[Penalty Weight]]*NightTimeDriveStefan[[#This Row],[Duration]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
@@ -3106,7 +3480,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{2691DD60-8F0D-4A00-BE27-FE334C07FAC0}" name="NightTimeDrive" displayName="NightTimeDrive" ref="E12:G14" totalsRowCount="1" headerRowDxfId="95" dataDxfId="93" totalsRowDxfId="91" headerRowBorderDxfId="94" tableBorderDxfId="92" totalsRowBorderDxfId="90">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{2691DD60-8F0D-4A00-BE27-FE334C07FAC0}" name="NightTimeDriveChristiaan" displayName="NightTimeDriveChristiaan" ref="E12:G14" totalsRowCount="1" headerRowDxfId="95" dataDxfId="93" totalsRowDxfId="91" headerRowBorderDxfId="94" tableBorderDxfId="92" totalsRowBorderDxfId="90">
   <autoFilter ref="E12:G13" xr:uid="{932FCD99-6FCF-4AE6-A66E-74A568E6D121}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -3118,7 +3492,7 @@
     </tableColumn>
     <tableColumn id="2" xr3:uid="{C181C36A-8D62-47D8-8D26-3B259CBE4530}" name="Duration" totalsRowFunction="sum" dataDxfId="87" totalsRowDxfId="86"/>
     <tableColumn id="3" xr3:uid="{904077CA-AF98-4510-BEF4-9B248A3A20F5}" name="Points" totalsRowFunction="sum" dataDxfId="85" totalsRowDxfId="84">
-      <calculatedColumnFormula>NightTimeDrive[[#This Row],[Penalty Weight]]*NightTimeDrive[[#This Row],[Duration]]</calculatedColumnFormula>
+      <calculatedColumnFormula>NightTimeDriveChristiaan[[#This Row],[Penalty Weight]]*NightTimeDriveChristiaan[[#This Row],[Duration]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
@@ -3170,19 +3544,19 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{5CE1FAFA-4CDE-4F06-804A-41746F5F5473}" name="NightTimeDrive11" displayName="NightTimeDrive11" ref="E12:G14" totalsRowCount="1" headerRowDxfId="62" dataDxfId="60" totalsRowDxfId="58" headerRowBorderDxfId="61" tableBorderDxfId="59" totalsRowBorderDxfId="57">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{07F85C93-6301-4631-9A07-A29BAEDC601A}" name="NightTimeDriveDerrick" displayName="NightTimeDriveDerrick" ref="E12:G14" totalsRowCount="1" headerRowDxfId="62" dataDxfId="60" totalsRowDxfId="58" headerRowBorderDxfId="61" tableBorderDxfId="59" totalsRowBorderDxfId="57">
   <autoFilter ref="E12:G13" xr:uid="{932FCD99-6FCF-4AE6-A66E-74A568E6D121}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{735D4564-3A90-415B-B47E-5EA90825A97A}" name="Penalty Weight" totalsRowLabel="Total" dataDxfId="56" totalsRowDxfId="55">
+    <tableColumn id="1" xr3:uid="{908B4C1D-4D0F-45BC-ADE7-4678CCD8016C}" name="Penalty Weight" totalsRowLabel="Total" dataDxfId="56" totalsRowDxfId="55">
       <calculatedColumnFormula>2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{EEF150EB-580C-474F-8688-6A037448742C}" name="Duration" totalsRowFunction="sum" dataDxfId="54" totalsRowDxfId="53"/>
-    <tableColumn id="3" xr3:uid="{5CEA56CD-422B-4282-AD7D-E4F69237A98B}" name="Points" totalsRowFunction="sum" dataDxfId="52" totalsRowDxfId="51">
-      <calculatedColumnFormula>NightTimeDrive11[[#This Row],[Penalty Weight]]*NightTimeDrive11[[#This Row],[Duration]]</calculatedColumnFormula>
+    <tableColumn id="2" xr3:uid="{686CE1C9-56A0-418C-A5F9-5428290550A7}" name="Duration" totalsRowFunction="sum" dataDxfId="54" totalsRowDxfId="53"/>
+    <tableColumn id="3" xr3:uid="{0303D504-DC81-435E-A6AF-FC40BFDF1A29}" name="Points" totalsRowFunction="sum" dataDxfId="52" totalsRowDxfId="51">
+      <calculatedColumnFormula>NightTimeDriveDerrick[[#This Row],[Penalty Weight]]*NightTimeDriveDerrick[[#This Row],[Duration]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
@@ -3190,7 +3564,7 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{66027C31-F46F-4630-BA7C-A7D788214406}" name="DistancePointsDerrick" displayName="DistancePointsDerrick" ref="L6:R13" totalsRowShown="0" headerRowDxfId="50" dataDxfId="48" headerRowBorderDxfId="49" tableBorderDxfId="47" totalsRowBorderDxfId="46">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{2B9BC8F6-98BE-4783-B971-02ABC492FDCC}" name="DistancePointsStefan45" displayName="DistancePointsStefan45" ref="L6:R13" totalsRowShown="0" headerRowDxfId="50" dataDxfId="48" headerRowBorderDxfId="49" tableBorderDxfId="47" totalsRowBorderDxfId="46">
   <autoFilter ref="L6:R13" xr:uid="{E011F3DC-4D15-4380-B07D-61D2F4291EE8}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -3201,20 +3575,20 @@
     <filterColumn colId="6" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{0276F9D3-B063-44DA-ADE6-1070BFDB3D35}" name="Lower" dataDxfId="45"/>
-    <tableColumn id="2" xr3:uid="{A553EDA2-505F-4944-960E-813BAE0280E6}" name="Upper" dataDxfId="44"/>
-    <tableColumn id="3" xr3:uid="{0D70A2B2-3135-468C-A321-4AEC2A2C9C11}" name="Blue" dataDxfId="43" dataCellStyle="Blue"/>
-    <tableColumn id="4" xr3:uid="{E8B32CB2-909D-40E6-8289-BAEBC5F6C299}" name="Bronze" dataDxfId="42" dataCellStyle="Bronze"/>
-    <tableColumn id="5" xr3:uid="{128F56E7-FA96-49D8-BA0E-6D47528F1475}" name="Silver" dataDxfId="41" dataCellStyle="Silver"/>
-    <tableColumn id="6" xr3:uid="{54B51153-77EB-4AD5-A4B1-A65717A58F23}" name="Gold" dataDxfId="40" dataCellStyle="Gold"/>
-    <tableColumn id="7" xr3:uid="{DCB5DC0A-9344-439A-829F-17C180815C46}" name="Diamond" dataDxfId="39" dataCellStyle="Diamond"/>
+    <tableColumn id="1" xr3:uid="{BE53131C-17AD-4665-A24B-6EBE0ABFD6F0}" name="Lower" dataDxfId="45"/>
+    <tableColumn id="2" xr3:uid="{1FF614C2-712A-495A-B0D1-1D4E5486D8B6}" name="Upper" dataDxfId="44"/>
+    <tableColumn id="3" xr3:uid="{4C9045D6-FECA-4036-883E-EE867CA64702}" name="Blue" dataDxfId="43" dataCellStyle="Blue"/>
+    <tableColumn id="4" xr3:uid="{01F199FF-7C53-4988-A952-1F8D27699DD6}" name="Bronze" dataDxfId="42" dataCellStyle="Bronze"/>
+    <tableColumn id="5" xr3:uid="{5DAD8ECE-EBBA-40EA-B838-268E75B3AD0D}" name="Silver" dataDxfId="41" dataCellStyle="Silver"/>
+    <tableColumn id="6" xr3:uid="{31E26907-9A2E-4870-BBE3-0D239AF42D23}" name="Gold" dataDxfId="40" dataCellStyle="Gold"/>
+    <tableColumn id="7" xr3:uid="{99D465DC-4820-4AB5-8ED7-03F7CEEB3D23}" name="Diamond" dataDxfId="39" dataCellStyle="Diamond"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{BA3552F5-BA84-40EA-9705-39CDD98F00E4}" name="DrivingStatusDerrick" displayName="DrivingStatusDerrick" ref="M26:Q31" totalsRowShown="0" headerRowDxfId="38" headerRowBorderDxfId="37" tableBorderDxfId="36" totalsRowBorderDxfId="35">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{C17754A1-2A22-478E-86EE-72ADFA47551C}" name="DrivingStatusStefan46" displayName="DrivingStatusStefan46" ref="M26:Q31" totalsRowShown="0" headerRowDxfId="38" headerRowBorderDxfId="37" tableBorderDxfId="36" totalsRowBorderDxfId="35">
   <autoFilter ref="M26:Q31" xr:uid="{DC26E8D9-5FBB-4486-917F-B1866C4C6343}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -3223,11 +3597,11 @@
     <filterColumn colId="4" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{421B8BD1-6ECD-4E7F-B4CC-3E6B400A6616}" name="Lower" dataDxfId="34" dataCellStyle="Silver"/>
-    <tableColumn id="2" xr3:uid="{AC79C6A7-9997-42DA-9554-F726645E1847}" name="Upper" dataDxfId="33" dataCellStyle="Silver"/>
-    <tableColumn id="3" xr3:uid="{86277536-AE35-4170-B2EE-720D4049918D}" name="Category" dataDxfId="32" dataCellStyle="Silver"/>
-    <tableColumn id="4" xr3:uid="{A9D36B79-51B1-4307-9F74-135ECAE6B10E}" name="Fuel %" dataDxfId="31" dataCellStyle="Silver"/>
-    <tableColumn id="5" xr3:uid="{177AEE58-7FAC-4322-86D6-2E43CB79763D}" name="Color" dataDxfId="30" dataCellStyle="Silver"/>
+    <tableColumn id="1" xr3:uid="{F60F2F47-4FE0-43F5-99B7-0E6CBA082ECE}" name="Lower" dataDxfId="34" dataCellStyle="Silver"/>
+    <tableColumn id="2" xr3:uid="{D9E0B627-C8F6-4A85-9C0E-82909016DD21}" name="Upper" dataDxfId="33" dataCellStyle="Silver"/>
+    <tableColumn id="3" xr3:uid="{9E2DCFD2-AF4E-42EB-8CC4-814F06C784B2}" name="Category" dataDxfId="32" dataCellStyle="Silver"/>
+    <tableColumn id="4" xr3:uid="{5CCE3F5D-7D82-45DD-999C-A09D15B06456}" name="Fuel %" dataDxfId="31" dataCellStyle="Silver"/>
+    <tableColumn id="5" xr3:uid="{CA9F0CC5-323E-474F-951B-6EFD4AABBBE6}" name="Color" dataDxfId="30" dataCellStyle="Silver"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -3530,12 +3904,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AB3F539-0250-415E-9699-09B43B836E74}">
-  <sheetPr>
+  <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="B2:AC33"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R3" sqref="R3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3566,7 +3942,7 @@
     <row r="2" spans="2:29" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="66" t="str">
         <f ca="1">_xlfn.CONCAT("Drive Summary ",J18, " ",TEXT(TODAY(), "mmmm yyyy"))</f>
-        <v>Drive Summary Stefan March 2025</v>
+        <v>Drive Summary Stefan April 2025</v>
       </c>
       <c r="C2" s="66"/>
       <c r="D2" s="66"/>
@@ -3594,7 +3970,7 @@
       <c r="D5"/>
       <c r="E5" s="16" t="str">
         <f ca="1">TEXT(TODAY(), "mmmm yyyy")</f>
-        <v>March 2025</v>
+        <v>April 2025</v>
       </c>
       <c r="F5" s="16" t="s">
         <v>1</v>
@@ -3624,18 +4000,18 @@
       </c>
       <c r="C6" s="7">
         <f>MIN(1500, IF($C$13,G7,G6+G9))</f>
-        <v>1500</v>
+        <v>1482</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F6" s="7">
         <f>J11</f>
-        <v>2000</v>
+        <v>1302</v>
       </c>
       <c r="G6" s="19">
         <f>J7</f>
-        <v>1489</v>
+        <v>1132</v>
       </c>
       <c r="I6" s="18" t="s">
         <v>30</v>
@@ -3682,17 +4058,17 @@
       </c>
       <c r="F7" s="7">
         <f>F6/J27*J26</f>
-        <v>2066.666666666667</v>
+        <v>1698.2608695652175</v>
       </c>
       <c r="G7" s="7">
         <f>G6/J27*J26</f>
-        <v>1538.6333333333332</v>
+        <v>1476.5217391304348</v>
       </c>
       <c r="I7" s="7" t="s">
         <v>0</v>
       </c>
       <c r="J7" s="7">
-        <v>1489</v>
+        <v>1132</v>
       </c>
       <c r="L7" s="13">
         <v>0</v>
@@ -3723,18 +4099,18 @@
       </c>
       <c r="C8" s="7">
         <f>IF( AND( J9&lt;=J24+J19, J9&gt;=J24-J19 ), J9, J24)</f>
-        <v>300</v>
+        <v>236</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F8" s="6">
         <f>F6/J27</f>
-        <v>66.666666666666671</v>
+        <v>56.608695652173914</v>
       </c>
       <c r="G8" s="6">
         <f>G6/J27</f>
-        <v>49.633333333333333</v>
+        <v>49.217391304347828</v>
       </c>
       <c r="I8" s="30" t="s">
         <v>4</v>
@@ -3770,24 +4146,24 @@
       </c>
       <c r="C9" s="7">
         <f>VLOOKUP(IF(C13,F7,F6),N17:P23,3)</f>
-        <v>100</v>
+        <v>300</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F9" s="7" t="str">
+      <c r="F9" s="7">
         <f>IF(J31&gt;=M13, "Unlimited", J31-F6)</f>
-        <v>Unlimited</v>
+        <v>497</v>
       </c>
       <c r="G9" s="7">
         <f>50*J28 + IF(J26&lt;30,(30-J26)*G8,0)</f>
-        <v>50</v>
+        <v>350</v>
       </c>
       <c r="I9" s="30" t="s">
         <v>27</v>
       </c>
       <c r="J9" s="7">
-        <v>300</v>
+        <v>236</v>
       </c>
       <c r="L9" s="13">
         <v>600</v>
@@ -3854,7 +4230,7 @@
       </c>
       <c r="C11" s="7">
         <f>SUM(C6:C10)</f>
-        <v>2500</v>
+        <v>2618</v>
       </c>
       <c r="E11" s="68" t="s">
         <v>27</v>
@@ -3865,7 +4241,7 @@
         <v>44</v>
       </c>
       <c r="J11" s="7">
-        <v>2000</v>
+        <v>1302</v>
       </c>
       <c r="L11" s="13">
         <v>1200</v>
@@ -3946,21 +4322,20 @@
         <v>0</v>
       </c>
       <c r="E13" s="1">
-        <f>2</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F13" s="1">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="G13" s="1">
-        <f>NightTimeDrive1114[[#This Row],[Penalty Weight]]*NightTimeDrive1114[[#This Row],[Duration]]</f>
-        <v>0</v>
+        <f>NightTimeDriveStefan[[#This Row],[Penalty Weight]]*NightTimeDriveStefan[[#This Row],[Duration]]</f>
+        <v>68</v>
       </c>
       <c r="I13" s="30" t="s">
         <v>20</v>
       </c>
       <c r="J13" s="30">
-        <v>2339.14</v>
+        <v>1169.75</v>
       </c>
       <c r="L13" s="14">
         <v>1800</v>
@@ -3993,18 +4368,18 @@
       </c>
       <c r="C14" s="37">
         <f>J13</f>
-        <v>2339.14</v>
+        <v>1169.75</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>47</v>
       </c>
       <c r="F14" s="1">
-        <f>SUBTOTAL(109,NightTimeDrive1114[Duration])</f>
-        <v>0</v>
+        <f>SUBTOTAL(109,NightTimeDriveStefan[Duration])</f>
+        <v>17</v>
       </c>
       <c r="G14" s="1">
-        <f>SUBTOTAL(109,NightTimeDrive1114[Points])</f>
-        <v>0</v>
+        <f>SUBTOTAL(109,NightTimeDriveStefan[Points])</f>
+        <v>68</v>
       </c>
       <c r="I14" s="7" t="s">
         <v>37</v>
@@ -4024,7 +4399,7 @@
       </c>
       <c r="C15" s="38" t="str">
         <f>_xlfn.CONCAT("Đ",J32*VLOOKUP(C12,O26:P31,2,FALSE)*10)</f>
-        <v>Đ11695.7</v>
+        <v>Đ5848.75</v>
       </c>
       <c r="D15" s="4"/>
       <c r="N15" s="68" t="str">
@@ -4047,7 +4422,7 @@
       </c>
       <c r="C16" s="37">
         <f>MAX(0,C11-C14)</f>
-        <v>160.86000000000013</v>
+        <v>1448.25</v>
       </c>
       <c r="I16" s="65" t="s">
         <v>38</v>
@@ -4125,7 +4500,7 @@
         <v>57</v>
       </c>
       <c r="J20" s="64">
-        <v>45747</v>
+        <v>45771</v>
       </c>
       <c r="N20" s="1">
         <v>900</v>
@@ -4185,8 +4560,8 @@
         <v>27</v>
       </c>
       <c r="J24" s="59">
-        <f>MAX(0,300-NightTimeDrive1114[[#Totals],[Points]])</f>
-        <v>300</v>
+        <f>MAX(0,300-NightTimeDriveStefan[[#Totals],[Points]])</f>
+        <v>232</v>
       </c>
     </row>
     <row r="25" spans="9:17" x14ac:dyDescent="0.25">
@@ -4208,11 +4583,11 @@
     <row r="26" spans="9:17" x14ac:dyDescent="0.25">
       <c r="I26" s="58" t="str">
         <f ca="1">_xlfn.CONCAT("Days ",TEXT(TODAY(), "mmm yyyy"))</f>
-        <v>Days Mar 2025</v>
+        <v>Days Apr 2025</v>
       </c>
       <c r="J26" s="61">
         <f>DAY(EOMONTH(J20, 0))</f>
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M26" s="18" t="s">
         <v>5</v>
@@ -4236,7 +4611,7 @@
       </c>
       <c r="J27" s="61">
         <f>DAY(J20)-1</f>
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="M27" s="39">
         <v>0</v>
@@ -4260,7 +4635,7 @@
       </c>
       <c r="J28" s="60">
         <f>J26-J27</f>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="M28" s="42">
         <v>800</v>
@@ -4284,7 +4659,7 @@
       </c>
       <c r="J29" s="62">
         <f>C11-VLOOKUP(C11,M27:O31,1,TRUE)</f>
-        <v>0</v>
+        <v>118</v>
       </c>
       <c r="M29" s="45">
         <v>1600</v>
@@ -4308,7 +4683,7 @@
       </c>
       <c r="J30" s="63">
         <f>MAX(0,C9-J29)</f>
-        <v>100</v>
+        <v>182</v>
       </c>
       <c r="M30" s="48">
         <v>2200</v>
@@ -4332,7 +4707,7 @@
       </c>
       <c r="J31" s="60" cm="1">
         <f t="array" ref="J31">MAX(_xlfn._xlws.FILTER(_xlfn.ANCHORARRAY(O17),_xlfn.ANCHORARRAY( P17)&gt;=J30))</f>
-        <v>1800</v>
+        <v>1799</v>
       </c>
       <c r="M31" s="52">
         <v>2500</v>
@@ -4356,7 +4731,7 @@
       </c>
       <c r="J32" s="7">
         <f>MIN(C14,C11)</f>
-        <v>2339.14</v>
+        <v>1169.75</v>
       </c>
     </row>
     <row r="33" spans="9:10" x14ac:dyDescent="0.25">
@@ -4365,7 +4740,7 @@
       </c>
       <c r="J33" s="7">
         <f>SUM(J7:J10,J12)</f>
-        <v>2589</v>
+        <v>2168</v>
       </c>
     </row>
   </sheetData>
@@ -4419,7 +4794,7 @@
       <formula>$J$14="Diamond"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="1">
+  <dataValidations disablePrompts="1" count="1">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The predicted status gives a realistic prediction of the driving status. If the prediction is disable, best case scenario is assumed, which is 50 point drive days and the distance remains in the same bracket." sqref="C13" xr:uid="{2B60514A-F1BD-4ADB-A95D-09E1CCF652F9}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4434,12 +4809,14 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F4D0580-2042-459B-AFBB-CAF4F016B905}">
-  <sheetPr>
+  <sheetPr codeName="Sheet2">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="B2:AC33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4470,7 +4847,7 @@
     <row r="2" spans="2:29" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="66" t="str">
         <f ca="1">_xlfn.CONCAT("Drive Summary ",J18, " ",TEXT(TODAY(), "mmmm yyyy"))</f>
-        <v>Drive Summary Christiaan March 2025</v>
+        <v>Drive Summary Christiaan April 2025</v>
       </c>
       <c r="C2" s="66"/>
       <c r="D2" s="66"/>
@@ -4498,7 +4875,7 @@
       <c r="D5"/>
       <c r="E5" s="16" t="str">
         <f ca="1">TEXT(TODAY(), "mmmm yyyy")</f>
-        <v>March 2025</v>
+        <v>April 2025</v>
       </c>
       <c r="F5" s="16" t="s">
         <v>1</v>
@@ -4528,17 +4905,18 @@
       </c>
       <c r="C6" s="7">
         <f>MIN(1500, IF($C$13,G7,G6+G9))</f>
-        <v>1500</v>
+        <v>1481</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F6" s="7">
-        <v>800</v>
+        <f>J11</f>
+        <v>255</v>
       </c>
       <c r="G6" s="19">
         <f>J7</f>
-        <v>1144</v>
+        <v>1131</v>
       </c>
       <c r="I6" s="18" t="s">
         <v>30</v>
@@ -4585,17 +4963,17 @@
       </c>
       <c r="F7" s="7">
         <f>F6/J27*J26</f>
-        <v>1078.2608695652173</v>
+        <v>332.60869565217394</v>
       </c>
       <c r="G7" s="7">
         <f>G6/J27*J26</f>
-        <v>1541.913043478261</v>
+        <v>1475.2173913043478</v>
       </c>
       <c r="I7" s="7" t="s">
         <v>0</v>
       </c>
       <c r="J7" s="7">
-        <v>1144</v>
+        <v>1131</v>
       </c>
       <c r="L7" s="13">
         <v>0</v>
@@ -4633,11 +5011,11 @@
       </c>
       <c r="F8" s="6">
         <f>F6/J27</f>
-        <v>34.782608695652172</v>
+        <v>11.086956521739131</v>
       </c>
       <c r="G8" s="6">
         <f>G6/J27</f>
-        <v>49.739130434782609</v>
+        <v>49.173913043478258</v>
       </c>
       <c r="I8" s="30" t="s">
         <v>4</v>
@@ -4673,18 +5051,18 @@
       </c>
       <c r="C9" s="7">
         <f>VLOOKUP(IF(C13,F7,F6),N17:P23,3)</f>
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F9" s="7" t="str">
+      <c r="F9" s="7">
         <f>IF(J31&gt;=M13, "Unlimited", J31-F6)</f>
-        <v>Unlimited</v>
+        <v>44</v>
       </c>
       <c r="G9" s="7">
         <f>50*J28 + IF(J26&lt;30,(30-J26)*G8,0)</f>
-        <v>400</v>
+        <v>350</v>
       </c>
       <c r="I9" s="30" t="s">
         <v>27</v>
@@ -4727,7 +5105,7 @@
         <v>11</v>
       </c>
       <c r="J10" s="30">
-        <v>125</v>
+        <v>300</v>
       </c>
       <c r="L10" s="13">
         <v>900</v>
@@ -4757,7 +5135,7 @@
       </c>
       <c r="C11" s="7">
         <f>SUM(C6:C10)</f>
-        <v>2450</v>
+        <v>2531</v>
       </c>
       <c r="E11" s="68" t="s">
         <v>27</v>
@@ -4768,7 +5146,7 @@
         <v>44</v>
       </c>
       <c r="J11" s="7">
-        <v>849</v>
+        <v>255</v>
       </c>
       <c r="L11" s="13">
         <v>1200</v>
@@ -4799,7 +5177,7 @@
       </c>
       <c r="C12" s="1" t="str">
         <f>VLOOKUP(C11,M27:O31,3,TRUE)</f>
-        <v>Gold</v>
+        <v>Diamond</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="16" t="s">
@@ -4856,14 +5234,14 @@
         <v>0</v>
       </c>
       <c r="G13" s="1">
-        <f>NightTimeDrive[[#This Row],[Penalty Weight]]*NightTimeDrive[[#This Row],[Duration]]</f>
+        <f>NightTimeDriveChristiaan[[#This Row],[Penalty Weight]]*NightTimeDriveChristiaan[[#This Row],[Duration]]</f>
         <v>0</v>
       </c>
       <c r="I13" s="30" t="s">
         <v>20</v>
       </c>
       <c r="J13" s="30">
-        <v>921.26</v>
+        <v>667.89</v>
       </c>
       <c r="L13" s="14">
         <v>1800</v>
@@ -4896,17 +5274,17 @@
       </c>
       <c r="C14" s="37">
         <f>J13</f>
-        <v>921.26</v>
+        <v>667.89</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>47</v>
       </c>
       <c r="F14" s="1">
-        <f>SUBTOTAL(109,NightTimeDrive[Duration])</f>
+        <f>SUBTOTAL(109,NightTimeDriveChristiaan[Duration])</f>
         <v>0</v>
       </c>
       <c r="G14" s="1">
-        <f>SUBTOTAL(109,NightTimeDrive[Points])</f>
+        <f>SUBTOTAL(109,NightTimeDriveChristiaan[Points])</f>
         <v>0</v>
       </c>
       <c r="I14" s="7" t="s">
@@ -4927,7 +5305,7 @@
       </c>
       <c r="C15" s="38" t="str">
         <f>_xlfn.CONCAT("Đ",J32*VLOOKUP(C12,O26:P31,2,FALSE)*10)</f>
-        <v>Đ3224.41</v>
+        <v>Đ3339.45</v>
       </c>
       <c r="D15" s="4"/>
       <c r="N15" s="68" t="str">
@@ -4950,7 +5328,7 @@
       </c>
       <c r="C16" s="37">
         <f>MAX(0,C11-C14)</f>
-        <v>1528.74</v>
+        <v>1863.1100000000001</v>
       </c>
       <c r="I16" s="68" t="s">
         <v>38</v>
@@ -5028,7 +5406,7 @@
         <v>57</v>
       </c>
       <c r="J20" s="64">
-        <v>45740</v>
+        <v>45771</v>
       </c>
       <c r="N20" s="1">
         <v>900</v>
@@ -5088,7 +5466,7 @@
         <v>27</v>
       </c>
       <c r="J24" s="59">
-        <f>MAX(0,300-NightTimeDrive1114[[#Totals],[Points]])</f>
+        <f>MAX(0,300-NightTimeDriveChristiaan[[#Totals],[Points]])</f>
         <v>300</v>
       </c>
     </row>
@@ -5111,11 +5489,11 @@
     <row r="26" spans="9:17" x14ac:dyDescent="0.25">
       <c r="I26" s="58" t="str">
         <f ca="1">_xlfn.CONCAT("Days ",TEXT(TODAY(), "mmm yyyy"))</f>
-        <v>Days Mar 2025</v>
+        <v>Days Apr 2025</v>
       </c>
       <c r="J26" s="61">
         <f>DAY(EOMONTH(J20, 0))</f>
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M26" s="18" t="s">
         <v>5</v>
@@ -5163,7 +5541,7 @@
       </c>
       <c r="J28" s="60">
         <f>J26-J27</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="M28" s="42">
         <v>800</v>
@@ -5187,7 +5565,7 @@
       </c>
       <c r="J29" s="62">
         <f>C11-VLOOKUP(C11,M27:O31,1,TRUE)</f>
-        <v>250</v>
+        <v>31</v>
       </c>
       <c r="M29" s="45">
         <v>1600</v>
@@ -5211,7 +5589,7 @@
       </c>
       <c r="J30" s="63">
         <f>MAX(0,C9-J29)</f>
-        <v>0</v>
+        <v>269</v>
       </c>
       <c r="M30" s="48">
         <v>2200</v>
@@ -5235,7 +5613,7 @@
       </c>
       <c r="J31" s="60" cm="1">
         <f t="array" ref="J31">MAX(_xlfn._xlws.FILTER(_xlfn.ANCHORARRAY(O17),_xlfn.ANCHORARRAY( P17)&gt;=J30))</f>
-        <v>1800</v>
+        <v>299</v>
       </c>
       <c r="M31" s="52">
         <v>2500</v>
@@ -5259,7 +5637,7 @@
       </c>
       <c r="J32" s="7">
         <f>MIN(C14,C11)</f>
-        <v>921.26</v>
+        <v>667.89</v>
       </c>
     </row>
     <row r="33" spans="9:10" x14ac:dyDescent="0.25">
@@ -5268,7 +5646,7 @@
       </c>
       <c r="J33" s="7">
         <f>SUM(J7:J10,J12)</f>
-        <v>2019</v>
+        <v>2181</v>
       </c>
     </row>
   </sheetData>
@@ -5336,13 +5714,15 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B3CC9EA-15F8-43BD-831E-AED1A6EDB8FC}">
-  <sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4033F0E9-CEA4-4A67-8E7A-E47961B6380D}">
+  <sheetPr codeName="Sheet5">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="B2:AC33"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5351,11 +5731,11 @@
     <col min="3" max="3" width="9.7109375" style="2" customWidth="1"/>
     <col min="4" max="4" width="2.7109375" style="2" customWidth="1"/>
     <col min="5" max="5" width="16.140625" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.7109375" style="2" customWidth="1"/>
     <col min="8" max="8" width="2.7109375" style="2" customWidth="1"/>
     <col min="9" max="9" width="22.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="2.7109375" style="2" customWidth="1"/>
     <col min="12" max="14" width="9.7109375" style="2" customWidth="1"/>
     <col min="15" max="15" width="10.5703125" style="2" customWidth="1"/>
@@ -5373,7 +5753,7 @@
     <row r="2" spans="2:29" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="66" t="str">
         <f ca="1">_xlfn.CONCAT("Drive Summary ",J18, " ",TEXT(TODAY(), "mmmm yyyy"))</f>
-        <v>Drive Summary Derrick March 2025</v>
+        <v>Drive Summary Derrick April 2025</v>
       </c>
       <c r="C2" s="66"/>
       <c r="D2" s="66"/>
@@ -5401,7 +5781,7 @@
       <c r="D5"/>
       <c r="E5" s="16" t="str">
         <f ca="1">TEXT(TODAY(), "mmmm yyyy")</f>
-        <v>March 2025</v>
+        <v>April 2025</v>
       </c>
       <c r="F5" s="16" t="s">
         <v>1</v>
@@ -5431,17 +5811,18 @@
       </c>
       <c r="C6" s="7">
         <f>MIN(1500, IF($C$13,G7,G6+G9))</f>
-        <v>1493</v>
+        <v>1498</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F6" s="7">
-        <v>500</v>
+        <f>J11</f>
+        <v>733</v>
       </c>
       <c r="G6" s="19">
         <f>J7</f>
-        <v>1093</v>
+        <v>1148</v>
       </c>
       <c r="I6" s="18" t="s">
         <v>30</v>
@@ -5480,7 +5861,7 @@
       </c>
       <c r="C7" s="7">
         <f>J8</f>
-        <v>150</v>
+        <v>300</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="1" t="s">
@@ -5488,17 +5869,17 @@
       </c>
       <c r="F7" s="7">
         <f>F6/J27*J26</f>
-        <v>673.91304347826087</v>
+        <v>956.08695652173913</v>
       </c>
       <c r="G7" s="7">
         <f>G6/J27*J26</f>
-        <v>1473.1739130434783</v>
+        <v>1497.391304347826</v>
       </c>
       <c r="I7" s="7" t="s">
         <v>0</v>
       </c>
       <c r="J7" s="7">
-        <v>1093</v>
+        <v>1148</v>
       </c>
       <c r="L7" s="13">
         <v>0</v>
@@ -5536,17 +5917,17 @@
       </c>
       <c r="F8" s="6">
         <f>F6/J27</f>
-        <v>21.739130434782609</v>
+        <v>31.869565217391305</v>
       </c>
       <c r="G8" s="6">
         <f>G6/J27</f>
-        <v>47.521739130434781</v>
+        <v>49.913043478260867</v>
       </c>
       <c r="I8" s="30" t="s">
         <v>4</v>
       </c>
       <c r="J8" s="7">
-        <v>150</v>
+        <v>300</v>
       </c>
       <c r="L8" s="13">
         <v>300</v>
@@ -5576,18 +5957,18 @@
       </c>
       <c r="C9" s="7">
         <f>VLOOKUP(IF(C13,F7,F6),N17:P23,3)</f>
-        <v>250</v>
+        <v>200</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F9" s="7" t="str">
+      <c r="F9" s="7">
         <f>IF(J31&gt;=M13, "Unlimited", J31-F6)</f>
-        <v>Unlimited</v>
+        <v>766</v>
       </c>
       <c r="G9" s="7">
         <f>50*J28 + IF(J26&lt;30,(30-J26)*G8,0)</f>
-        <v>400</v>
+        <v>350</v>
       </c>
       <c r="I9" s="30" t="s">
         <v>27</v>
@@ -5630,7 +6011,7 @@
         <v>11</v>
       </c>
       <c r="J10" s="30">
-        <v>250</v>
+        <v>200</v>
       </c>
       <c r="L10" s="13">
         <v>900</v>
@@ -5660,7 +6041,7 @@
       </c>
       <c r="C11" s="7">
         <f>SUM(C6:C10)</f>
-        <v>2493</v>
+        <v>2598</v>
       </c>
       <c r="E11" s="68" t="s">
         <v>27</v>
@@ -5671,7 +6052,7 @@
         <v>44</v>
       </c>
       <c r="J11" s="7">
-        <v>524</v>
+        <v>733</v>
       </c>
       <c r="L11" s="13">
         <v>1200</v>
@@ -5702,7 +6083,7 @@
       </c>
       <c r="C12" s="1" t="str">
         <f>VLOOKUP(C11,M27:O31,3,TRUE)</f>
-        <v>Gold</v>
+        <v>Diamond</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="16" t="s">
@@ -5759,14 +6140,14 @@
         <v>0</v>
       </c>
       <c r="G13" s="1">
-        <f>NightTimeDrive11[[#This Row],[Penalty Weight]]*NightTimeDrive11[[#This Row],[Duration]]</f>
+        <f>NightTimeDriveDerrick[[#This Row],[Penalty Weight]]*NightTimeDriveDerrick[[#This Row],[Duration]]</f>
         <v>0</v>
       </c>
       <c r="I13" s="30" t="s">
         <v>20</v>
       </c>
       <c r="J13" s="30">
-        <v>0</v>
+        <v>660.9</v>
       </c>
       <c r="L13" s="14">
         <v>1800</v>
@@ -5799,17 +6180,17 @@
       </c>
       <c r="C14" s="37">
         <f>J13</f>
-        <v>0</v>
+        <v>660.9</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>47</v>
       </c>
       <c r="F14" s="1">
-        <f>SUBTOTAL(109,NightTimeDrive11[Duration])</f>
+        <f>SUBTOTAL(109,NightTimeDriveDerrick[Duration])</f>
         <v>0</v>
       </c>
       <c r="G14" s="1">
-        <f>SUBTOTAL(109,NightTimeDrive11[Points])</f>
+        <f>SUBTOTAL(109,NightTimeDriveDerrick[Points])</f>
         <v>0</v>
       </c>
       <c r="I14" s="7" t="s">
@@ -5830,7 +6211,7 @@
       </c>
       <c r="C15" s="38" t="str">
         <f>_xlfn.CONCAT("Đ",J32*VLOOKUP(C12,O26:P31,2,FALSE)*10)</f>
-        <v>Đ0</v>
+        <v>Đ3304.5</v>
       </c>
       <c r="D15" s="4"/>
       <c r="N15" s="68" t="str">
@@ -5853,7 +6234,7 @@
       </c>
       <c r="C16" s="37">
         <f>MAX(0,C11-C14)</f>
-        <v>2493</v>
+        <v>1937.1</v>
       </c>
       <c r="I16" s="65" t="s">
         <v>38</v>
@@ -5880,15 +6261,15 @@
         <v>31</v>
       </c>
       <c r="N17" s="1" cm="1">
-        <f t="array" ref="N17:N23">DistancePointsDerrick[Lower]</f>
+        <f t="array" ref="N17:N23">DistancePointsStefan45[Lower]</f>
         <v>0</v>
       </c>
       <c r="O17" s="1" cm="1">
-        <f t="array" ref="O17:O23">DistancePointsDerrick[Upper]</f>
+        <f t="array" ref="O17:O23">DistancePointsStefan45[Upper]</f>
         <v>299</v>
       </c>
       <c r="P17" s="1" cm="1">
-        <f t="array" ref="P17:P23">_xlfn.XLOOKUP(J14,DistancePointsDerrick[#Headers],DistancePointsDerrick[])</f>
+        <f t="array" ref="P17:P23">_xlfn.XLOOKUP(J14,DistancePointsStefan45[#Headers],DistancePointsStefan45[])</f>
         <v>300</v>
       </c>
     </row>
@@ -5931,7 +6312,7 @@
         <v>57</v>
       </c>
       <c r="J20" s="64">
-        <v>45740</v>
+        <v>45771</v>
       </c>
       <c r="N20" s="1">
         <v>900</v>
@@ -5991,7 +6372,7 @@
         <v>27</v>
       </c>
       <c r="J24" s="59">
-        <f>MAX(0,300-NightTimeDrive1114[[#Totals],[Points]])</f>
+        <f>MAX(0,300-NightTimeDriveDerrick[[#Totals],[Points]])</f>
         <v>300</v>
       </c>
     </row>
@@ -6014,11 +6395,11 @@
     <row r="26" spans="9:17" x14ac:dyDescent="0.25">
       <c r="I26" s="58" t="str">
         <f ca="1">_xlfn.CONCAT("Days ",TEXT(TODAY(), "mmm yyyy"))</f>
-        <v>Days Mar 2025</v>
+        <v>Days Apr 2025</v>
       </c>
       <c r="J26" s="61">
         <f>DAY(EOMONTH(J20, 0))</f>
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M26" s="18" t="s">
         <v>5</v>
@@ -6066,7 +6447,7 @@
       </c>
       <c r="J28" s="60">
         <f>J26-J27</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="M28" s="42">
         <v>800</v>
@@ -6090,7 +6471,7 @@
       </c>
       <c r="J29" s="62">
         <f>C11-VLOOKUP(C11,M27:O31,1,TRUE)</f>
-        <v>293</v>
+        <v>98</v>
       </c>
       <c r="M29" s="45">
         <v>1600</v>
@@ -6114,7 +6495,7 @@
       </c>
       <c r="J30" s="63">
         <f>MAX(0,C9-J29)</f>
-        <v>0</v>
+        <v>102</v>
       </c>
       <c r="M30" s="48">
         <v>2200</v>
@@ -6138,7 +6519,7 @@
       </c>
       <c r="J31" s="60" cm="1">
         <f t="array" ref="J31">MAX(_xlfn._xlws.FILTER(_xlfn.ANCHORARRAY(O17),_xlfn.ANCHORARRAY( P17)&gt;=J30))</f>
-        <v>1800</v>
+        <v>1499</v>
       </c>
       <c r="M31" s="52">
         <v>2500</v>
@@ -6162,7 +6543,7 @@
       </c>
       <c r="J32" s="7">
         <f>MIN(C14,C11)</f>
-        <v>0</v>
+        <v>660.9</v>
       </c>
     </row>
     <row r="33" spans="9:10" x14ac:dyDescent="0.25">
@@ -6171,13 +6552,13 @@
       </c>
       <c r="J33" s="7">
         <f>SUM(J7:J10,J12)</f>
-        <v>2093</v>
+        <v>2248</v>
       </c>
     </row>
   </sheetData>
   <protectedRanges>
     <protectedRange sqref="C7:C8 C10 C16 C14" name="RequiresInput_1"/>
-    <protectedRange sqref="F6:G6" name="RequiresInput_1_1_1"/>
+    <protectedRange sqref="F6:G6" name="RequiresInput_1_1"/>
   </protectedRanges>
   <dataConsolidate/>
   <mergeCells count="9">
@@ -6225,8 +6606,8 @@
       <formula>$J$14="Diamond"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations disablePrompts="1" count="1">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The predicted status gives a realistic prediction of the driving status. If the prediction is disable, best case scenario is assumed, which is 50 point drive days and the distance remains in the same bracket." sqref="C13" xr:uid="{8E72BB58-1177-473B-BF7A-A98C86835AA3}"/>
+  <dataValidations count="1">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The predicted status gives a realistic prediction of the driving status. If the prediction is disable, best case scenario is assumed, which is 50 point drive days and the distance remains in the same bracket." sqref="C13" xr:uid="{B0F9DF6F-FAA0-43BD-8837-DEDA84525B23}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="32" orientation="portrait" r:id="rId1"/>

</xml_diff>